<commit_message>
update extraction processes with new data
</commit_message>
<xml_diff>
--- a/manual-extract/NewVars.xlsx
+++ b/manual-extract/NewVars.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="174">
   <si>
     <t>age</t>
   </si>
@@ -177,9 +177,6 @@
     <t>hhsize</t>
   </si>
   <si>
-    <t>HV009</t>
-  </si>
-  <si>
     <t>v136</t>
   </si>
   <si>
@@ -195,15 +192,9 @@
     <t>wealth_factor</t>
   </si>
   <si>
-    <t>HV270</t>
-  </si>
-  <si>
     <t>v190</t>
   </si>
   <si>
-    <t>HV271</t>
-  </si>
-  <si>
     <t>v191</t>
   </si>
   <si>
@@ -228,9 +219,6 @@
     <t>sex</t>
   </si>
   <si>
-    <t>HC27</t>
-  </si>
-  <si>
     <t>b4</t>
   </si>
   <si>
@@ -243,9 +231,6 @@
     <t>breast_duration</t>
   </si>
   <si>
-    <t>M4</t>
-  </si>
-  <si>
     <t>m4</t>
   </si>
   <si>
@@ -291,9 +276,6 @@
     <t>watersource</t>
   </si>
   <si>
-    <t>HV201</t>
-  </si>
-  <si>
     <t>v113</t>
   </si>
   <si>
@@ -457,13 +439,112 @@
   </si>
   <si>
     <t>v034</t>
+  </si>
+  <si>
+    <t>hc1</t>
+  </si>
+  <si>
+    <t>hc3</t>
+  </si>
+  <si>
+    <t>hc2</t>
+  </si>
+  <si>
+    <t>hv204</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>hc27</t>
+  </si>
+  <si>
+    <t>hv009</t>
+  </si>
+  <si>
+    <t>hv270</t>
+  </si>
+  <si>
+    <t>hv271</t>
+  </si>
+  <si>
+    <t>hv201</t>
+  </si>
+  <si>
+    <t>PR</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>integer</t>
+  </si>
+  <si>
+    <t>hc10</t>
+  </si>
+  <si>
+    <t>hc12</t>
+  </si>
+  <si>
+    <t>hc15</t>
+  </si>
+  <si>
+    <t>character</t>
+  </si>
+  <si>
+    <t>hc4</t>
+  </si>
+  <si>
+    <t>hc56</t>
+  </si>
+  <si>
+    <t>hc57</t>
+  </si>
+  <si>
+    <t>hc6</t>
+  </si>
+  <si>
+    <t>hc61</t>
+  </si>
+  <si>
+    <t>hc7</t>
+  </si>
+  <si>
+    <t>hc73</t>
+  </si>
+  <si>
+    <t>hc9</t>
+  </si>
+  <si>
+    <t>hv002</t>
+  </si>
+  <si>
+    <t>hv003</t>
+  </si>
+  <si>
+    <t>hv014</t>
+  </si>
+  <si>
+    <t>hv035</t>
+  </si>
+  <si>
+    <t>hv101</t>
+  </si>
+  <si>
+    <t>hv104</t>
+  </si>
+  <si>
+    <t>hv105</t>
+  </si>
+  <si>
+    <t>hc62</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -483,16 +564,317 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Cambria"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -500,12 +882,160 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -529,10 +1059,52 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="43">
+    <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="24" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="28" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="32" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="36" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="40" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="21" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="25" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="29" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="33" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="37" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="41" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="22" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="26" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="30" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="34" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="38" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="42" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="19" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="23" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="27" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="31" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="35" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="39" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="8" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="12" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="14" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="17" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="7" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="3" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="4" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="5" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="6" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="10" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="13" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="9" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Note" xfId="16" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="11" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="2" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="18" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="15" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -833,9 +1405,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F23" sqref="F23"/>
+      <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -891,6 +1463,7 @@
       <c r="F2" s="3" t="s">
         <v>47</v>
       </c>
+      <c r="G2" s="23"/>
     </row>
     <row r="3" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
@@ -905,6 +1478,7 @@
       <c r="F3" s="3" t="s">
         <v>49</v>
       </c>
+      <c r="G3" s="23"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -919,9 +1493,13 @@
       <c r="D4" t="s">
         <v>15</v>
       </c>
+      <c r="E4" t="s">
+        <v>141</v>
+      </c>
       <c r="F4" t="s">
-        <v>132</v>
-      </c>
+        <v>126</v>
+      </c>
+      <c r="G4" s="23"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -936,9 +1514,13 @@
       <c r="D5" t="s">
         <v>12</v>
       </c>
+      <c r="E5" t="s">
+        <v>142</v>
+      </c>
       <c r="F5" t="s">
-        <v>134</v>
-      </c>
+        <v>128</v>
+      </c>
+      <c r="G5" s="23"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -953,9 +1535,13 @@
       <c r="D6" t="s">
         <v>13</v>
       </c>
+      <c r="E6" t="s">
+        <v>143</v>
+      </c>
       <c r="F6" t="s">
-        <v>133</v>
-      </c>
+        <v>127</v>
+      </c>
+      <c r="G6" s="23"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -964,6 +1550,10 @@
       <c r="B7" t="s">
         <v>17</v>
       </c>
+      <c r="E7" t="s">
+        <v>145</v>
+      </c>
+      <c r="G7" s="23"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -972,6 +1562,10 @@
       <c r="B8" t="s">
         <v>18</v>
       </c>
+      <c r="E8" t="s">
+        <v>145</v>
+      </c>
+      <c r="G8" s="23"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -980,6 +1574,10 @@
       <c r="B9" t="s">
         <v>19</v>
       </c>
+      <c r="E9" t="s">
+        <v>145</v>
+      </c>
+      <c r="G9" s="23"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -994,6 +1592,7 @@
       <c r="F10" s="1" t="s">
         <v>31</v>
       </c>
+      <c r="G10" s="23"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -1008,6 +1607,7 @@
       <c r="F11" s="4" t="s">
         <v>35</v>
       </c>
+      <c r="G11" s="23"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -1022,6 +1622,7 @@
       <c r="F12" s="2" t="s">
         <v>33</v>
       </c>
+      <c r="G12" s="23"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -1031,11 +1632,12 @@
         <v>23</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>64</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="G13" s="23"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -1045,11 +1647,12 @@
         <v>24</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>66</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="G14" s="23"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -1059,246 +1662,308 @@
         <v>25</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>68</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="G15" s="23"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>26</v>
       </c>
       <c r="B16" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>70</v>
+        <v>146</v>
       </c>
       <c r="F16" s="12" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+      <c r="G16" s="23"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
         <v>26</v>
       </c>
       <c r="B17" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C17" t="s">
-        <v>73</v>
+        <v>69</v>
+      </c>
+      <c r="E17" t="s">
+        <v>145</v>
       </c>
       <c r="F17" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+      <c r="G17" s="23"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
         <v>26</v>
       </c>
       <c r="B18" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C18" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D18" t="s">
         <v>15</v>
       </c>
       <c r="E18" s="13" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="F18" s="13" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+      <c r="G18" s="23"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
         <v>26</v>
       </c>
       <c r="B19" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="E19" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="F19" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+        <v>136</v>
+      </c>
+      <c r="G19" s="23"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
         <v>26</v>
       </c>
       <c r="B20" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="E20" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="F20" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+      <c r="G20" s="23"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
         <v>26</v>
       </c>
       <c r="B21" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="E21" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="F21" s="15" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+      <c r="G21" s="23"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="14" t="s">
         <v>26</v>
       </c>
       <c r="B22" t="s">
-        <v>88</v>
+        <v>83</v>
+      </c>
+      <c r="E22" t="s">
+        <v>145</v>
       </c>
       <c r="F22" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+      <c r="G22" s="23"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
         <v>26</v>
       </c>
       <c r="B23" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+      <c r="E23" t="s">
+        <v>145</v>
+      </c>
+      <c r="G23" s="23"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="14" t="s">
         <v>26</v>
       </c>
       <c r="B24" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+      <c r="E24" t="s">
+        <v>145</v>
+      </c>
+      <c r="G24" s="23"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="14" t="s">
         <v>26</v>
       </c>
       <c r="B25" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="C25" t="s">
-        <v>100</v>
+        <v>94</v>
+      </c>
+      <c r="E25" t="s">
+        <v>145</v>
       </c>
       <c r="F25" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+      <c r="G25" s="23"/>
+    </row>
+    <row r="26" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B26" s="14" t="s">
-        <v>112</v>
+        <v>106</v>
+      </c>
+      <c r="E26" s="14" t="s">
+        <v>50</v>
       </c>
       <c r="F26" s="16" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G26" s="23"/>
+    </row>
+    <row r="27" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>128</v>
+        <v>122</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>145</v>
       </c>
       <c r="F27" s="21" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+      <c r="G27" s="23"/>
+    </row>
+    <row r="28" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>129</v>
+        <v>123</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>145</v>
       </c>
       <c r="F28" s="21" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+      <c r="G28" s="23"/>
+    </row>
+    <row r="29" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B29" s="14" t="s">
-        <v>113</v>
+        <v>107</v>
+      </c>
+      <c r="E29" s="14" t="s">
+        <v>145</v>
       </c>
       <c r="F29" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+      <c r="G29" s="23"/>
+    </row>
+    <row r="30" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B30" s="14" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="D30" s="14" t="s">
-        <v>123</v>
+        <v>117</v>
+      </c>
+      <c r="E30" s="14" t="s">
+        <v>145</v>
       </c>
       <c r="F30" s="14" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+      <c r="G30" s="23"/>
+    </row>
+    <row r="31" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>138</v>
+        <v>132</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>145</v>
       </c>
       <c r="F31" s="21" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+      <c r="G31" s="23"/>
+    </row>
+    <row r="32" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>139</v>
+        <v>133</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>145</v>
       </c>
       <c r="F32" s="21" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+      <c r="G32" s="23"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>28</v>
       </c>
       <c r="B33" t="s">
-        <v>105</v>
+        <v>99</v>
+      </c>
+      <c r="E33" t="s">
+        <v>145</v>
       </c>
       <c r="F33" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+      <c r="G33" s="23"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>28</v>
       </c>
       <c r="B34" t="s">
         <v>39</v>
       </c>
+      <c r="E34" t="s">
+        <v>145</v>
+      </c>
       <c r="F34" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G34" s="23"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="14" t="s">
         <v>28</v>
       </c>
@@ -1306,174 +1971,221 @@
         <v>52</v>
       </c>
       <c r="E35" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="F35" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="F35" s="7" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G35" s="23"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="14" t="s">
         <v>28</v>
       </c>
       <c r="B36" t="s">
+        <v>54</v>
+      </c>
+      <c r="E36" t="s">
         <v>55</v>
       </c>
-      <c r="E36" t="s">
-        <v>56</v>
-      </c>
       <c r="F36" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+      <c r="G36" s="23"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="14" t="s">
         <v>28</v>
       </c>
       <c r="B37" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E37" s="8" t="s">
-        <v>59</v>
+        <v>148</v>
       </c>
       <c r="F37" s="8" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+      <c r="G37" s="23"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="14" t="s">
         <v>28</v>
       </c>
       <c r="B38" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E38" s="8" t="s">
-        <v>61</v>
+        <v>149</v>
       </c>
       <c r="F38" s="8" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+      <c r="G38" s="23"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="14" t="s">
         <v>28</v>
       </c>
       <c r="B39" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="E39" s="14" t="s">
-        <v>91</v>
+        <v>150</v>
       </c>
       <c r="F39" s="14" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" s="18" customFormat="1" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+      <c r="G39" s="23"/>
+    </row>
+    <row r="40" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="18" t="s">
         <v>28</v>
       </c>
       <c r="B40" s="18" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="D40" s="18" t="s">
-        <v>118</v>
+        <v>112</v>
+      </c>
+      <c r="E40" s="18" t="s">
+        <v>144</v>
       </c>
       <c r="F40" s="22" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+      <c r="G40" s="23"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="14" t="s">
         <v>28</v>
       </c>
       <c r="B41" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="C41" t="s">
-        <v>116</v>
+        <v>110</v>
+      </c>
+      <c r="E41" t="s">
+        <v>145</v>
       </c>
       <c r="F41" s="19" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+      <c r="G41" s="23"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="14" t="s">
         <v>28</v>
       </c>
       <c r="B42" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C42" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+      <c r="E42" t="s">
+        <v>145</v>
+      </c>
+      <c r="G42" s="23"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="14" t="s">
         <v>28</v>
       </c>
       <c r="B43" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="E43" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="F43" s="17" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+      <c r="G43" s="23"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="14" t="s">
         <v>28</v>
       </c>
       <c r="B44" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="E44" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="F44" s="22" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+      <c r="G44" s="23"/>
+    </row>
+    <row r="45" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="14" t="s">
         <v>28</v>
       </c>
       <c r="B45" s="14" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="C45" s="14" t="s">
-        <v>108</v>
+        <v>102</v>
+      </c>
+      <c r="E45" s="14" t="s">
+        <v>145</v>
       </c>
       <c r="F45" s="14" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+      <c r="G45" s="23"/>
+    </row>
+    <row r="46" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="14" t="s">
         <v>28</v>
       </c>
       <c r="B46" s="14" t="s">
-        <v>110</v>
+        <v>104</v>
+      </c>
+      <c r="E46" s="14" t="s">
+        <v>145</v>
       </c>
       <c r="F46" s="14" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+      <c r="G46" s="23"/>
+    </row>
+    <row r="47" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="14" t="s">
         <v>28</v>
       </c>
       <c r="B47" s="14" t="s">
-        <v>120</v>
+        <v>114</v>
+      </c>
+      <c r="E47" s="14" t="s">
+        <v>145</v>
       </c>
       <c r="F47" s="14" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="49" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+      <c r="G47" s="23"/>
+    </row>
+    <row r="48" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E48" s="14" t="s">
+        <v>145</v>
+      </c>
+      <c r="G48" s="23"/>
+    </row>
+    <row r="49" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E49" s="14" t="s">
+        <v>145</v>
+      </c>
+      <c r="G49" s="23"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E50" t="s">
+        <v>145</v>
+      </c>
+      <c r="G50" s="23"/>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>29</v>
       </c>
@@ -1486,8 +2198,9 @@
       <c r="F51" s="5" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G51" s="23"/>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="14" t="s">
         <v>29</v>
       </c>
@@ -1500,8 +2213,9 @@
       <c r="F52" s="6" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G52" s="23"/>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="14" t="s">
         <v>29</v>
       </c>
@@ -1514,43 +2228,54 @@
       <c r="F53" s="3" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G53" s="23"/>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="14" t="s">
         <v>29</v>
       </c>
       <c r="B54" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+      <c r="E54" t="s">
+        <v>145</v>
+      </c>
+      <c r="G54" s="18"/>
+    </row>
+    <row r="55" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
         <v>29</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+      <c r="E55" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="G55" s="18"/>
+    </row>
+    <row r="56" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
         <v>29</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" s="3" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+      <c r="G56" s="18"/>
+    </row>
+    <row r="57" spans="1:7" s="3" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
         <v>29</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="59" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="60" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="61" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+        <v>120</v>
+      </c>
+      <c r="G57" s="18"/>
+    </row>
+    <row r="58" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="59" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="60" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="61" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1559,12 +2284,389 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B48"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B48"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="23" t="s">
+        <v>151</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="23" t="s">
+        <v>141</v>
+      </c>
+      <c r="B2" s="23" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="23" t="s">
+        <v>154</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="23" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="23" t="s">
+        <v>155</v>
+      </c>
+      <c r="B5" s="23" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="23" t="s">
+        <v>156</v>
+      </c>
+      <c r="B6" s="23" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="23" t="s">
+        <v>143</v>
+      </c>
+      <c r="B7" s="23" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="23" t="s">
+        <v>146</v>
+      </c>
+      <c r="B8" s="23" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="B9" s="23" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="23" t="s">
+        <v>158</v>
+      </c>
+      <c r="B10" s="23" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="23" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="23" t="s">
+        <v>159</v>
+      </c>
+      <c r="B12" s="23" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="23" t="s">
+        <v>160</v>
+      </c>
+      <c r="B13" s="23" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="23" t="s">
+        <v>161</v>
+      </c>
+      <c r="B14" s="23" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="B15" s="23" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="B16" s="23" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="23" t="s">
+        <v>163</v>
+      </c>
+      <c r="B17" s="23" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="B18" s="23" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="B19" s="23" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="B20" s="23" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="23" t="s">
+        <v>164</v>
+      </c>
+      <c r="B21" s="23" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22" s="23" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="23" t="s">
+        <v>165</v>
+      </c>
+      <c r="B23" s="23" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="23" t="s">
+        <v>99</v>
+      </c>
+      <c r="B24" s="23" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="B25" s="23" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="B26" s="23" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="23" t="s">
+        <v>166</v>
+      </c>
+      <c r="B27" s="23" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="23" t="s">
+        <v>167</v>
+      </c>
+      <c r="B28" s="23" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="B29" s="23" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="B30" s="23" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="23" t="s">
+        <v>147</v>
+      </c>
+      <c r="B31" s="23" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="23" t="s">
+        <v>168</v>
+      </c>
+      <c r="B32" s="23" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="B33" s="23" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="23" t="s">
+        <v>169</v>
+      </c>
+      <c r="B34" s="23" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="23" t="s">
+        <v>170</v>
+      </c>
+      <c r="B35" s="23" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="23" t="s">
+        <v>171</v>
+      </c>
+      <c r="B36" s="23" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="23" t="s">
+        <v>172</v>
+      </c>
+      <c r="B37" s="23" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="23" t="s">
+        <v>150</v>
+      </c>
+      <c r="B38" s="23" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="23" t="s">
+        <v>148</v>
+      </c>
+      <c r="B39" s="23" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="23" t="s">
+        <v>149</v>
+      </c>
+      <c r="B40" s="23" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="23" t="s">
+        <v>137</v>
+      </c>
+      <c r="B41" s="23" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="23" t="s">
+        <v>138</v>
+      </c>
+      <c r="B42" s="23" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="B43" s="23" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="23" t="s">
+        <v>71</v>
+      </c>
+      <c r="B44" s="23"/>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="B45" s="23"/>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="23" t="s">
+        <v>173</v>
+      </c>
+      <c r="B46" s="23"/>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="B47" s="23"/>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="B48" s="23"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1585,10 +2687,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C1" t="str">
         <f>CONCATENATE(A1, "=", B1, ",")</f>
@@ -1597,10 +2699,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C2" s="3" t="str">
         <f t="shared" ref="C2:C36" si="0">CONCATENATE(A2, "=", B2, ",")</f>
@@ -1609,10 +2711,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C3" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1621,10 +2723,10 @@
     </row>
     <row r="4" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="C4" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1645,10 +2747,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="B6" s="22" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="C6" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1657,10 +2759,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="C7" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1669,10 +2771,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="C8" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1684,7 +2786,7 @@
         <v>0</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="C9" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1708,7 +2810,7 @@
         <v>6</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="C11" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1720,7 +2822,7 @@
         <v>1</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C12" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1744,7 +2846,7 @@
         <v>23</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C14" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1756,7 +2858,7 @@
         <v>25</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C15" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1768,7 +2870,7 @@
         <v>24</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C16" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1789,10 +2891,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C18" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1801,10 +2903,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C19" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1813,10 +2915,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="C20" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1825,10 +2927,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C21" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1837,10 +2939,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="C22" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1873,7 +2975,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="B25" s="21" t="s">
         <v>51</v>
@@ -1885,10 +2987,10 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="B26" s="21" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="C26" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1897,10 +2999,10 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="B27" s="21" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="C27" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1909,10 +3011,10 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="C28" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1921,10 +3023,10 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="C29" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1933,10 +3035,10 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="C30" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1945,10 +3047,10 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="B31" s="22" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="C31" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1957,10 +3059,10 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="C32" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1972,7 +3074,7 @@
         <v>52</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C33" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1981,10 +3083,10 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B34" s="22" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="C34" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1993,10 +3095,10 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C35" s="3" t="str">
         <f t="shared" si="0"/>
@@ -2005,10 +3107,10 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C36" s="3" t="str">
         <f t="shared" si="0"/>
@@ -2032,52 +3134,52 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
@@ -2106,22 +3208,22 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finished variable cleaning. COMPLETE DHS DATASET
</commit_message>
<xml_diff>
--- a/manual-extract/NewVars.xlsx
+++ b/manual-extract/NewVars.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="180" windowWidth="27795" windowHeight="12525"/>
+    <workbookView xWindow="480" yWindow="240" windowWidth="27795" windowHeight="12465"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="249">
   <si>
     <t>age</t>
   </si>
@@ -600,18 +600,12 @@
     <t>hv205</t>
   </si>
   <si>
-    <t>calculate</t>
-  </si>
-  <si>
     <t>interview_month</t>
   </si>
   <si>
     <t>interview_year</t>
   </si>
   <si>
-    <t>fathers_age</t>
-  </si>
-  <si>
     <t>GE</t>
   </si>
   <si>
@@ -624,15 +618,9 @@
     <t>seq(1980, 2016)</t>
   </si>
   <si>
-    <t>seq(1200, 1800)</t>
-  </si>
-  <si>
     <t>seq(0, 59)</t>
   </si>
   <si>
-    <t>200 &lt; x &lt; 2000</t>
-  </si>
-  <si>
     <t>15 &lt; x &lt; 400</t>
   </si>
   <si>
@@ -645,18 +633,12 @@
     <t>c("Male", "Female")</t>
   </si>
   <si>
-    <t>c("Son/daughter", "Grandchild", "Brother/sister", "Other relative", "Adopted/foster child", "Not related")</t>
-  </si>
-  <si>
     <t>seq(1, 20)</t>
   </si>
   <si>
     <t>c('No', 'Yes')</t>
   </si>
   <si>
-    <t>seq(1, 50)</t>
-  </si>
-  <si>
     <t>c("Urban", "Rural")</t>
   </si>
   <si>
@@ -681,9 +663,6 @@
     <t>hv202</t>
   </si>
   <si>
-    <t>c("Pipe", "Tube Well", "Surface Water", "Rainwater", "Purchased", "Other")</t>
-  </si>
-  <si>
     <t>Drinking Water Sources</t>
   </si>
   <si>
@@ -711,9 +690,6 @@
     <t>hv108</t>
   </si>
   <si>
-    <t>c("No", "24hours", "2weeks")</t>
-  </si>
-  <si>
     <t>toilet</t>
   </si>
   <si>
@@ -730,13 +706,70 @@
   </si>
   <si>
     <t>hv105 &gt; 14 &amp; hv105 &lt; 66 for household</t>
+  </si>
+  <si>
+    <t>was the child ever breastfed?</t>
+  </si>
+  <si>
+    <t>ever_breastfed</t>
+  </si>
+  <si>
+    <t>derived from m5</t>
+  </si>
+  <si>
+    <t>seq(1, 40)</t>
+  </si>
+  <si>
+    <t>father_age</t>
+  </si>
+  <si>
+    <t>seq(0, 25)</t>
+  </si>
+  <si>
+    <t>seq(10,97)</t>
+  </si>
+  <si>
+    <t>seq(100, 2000)</t>
+  </si>
+  <si>
+    <t>seq(1, 75)</t>
+  </si>
+  <si>
+    <t>character(12)</t>
+  </si>
+  <si>
+    <t>seq(0, 30)</t>
+  </si>
+  <si>
+    <t>mother_age</t>
+  </si>
+  <si>
+    <t>seq(10, 96)</t>
+  </si>
+  <si>
+    <t>c("Pipe", "Tube Well", "Surface Water", "Rainwater", "Purchased")</t>
+  </si>
+  <si>
+    <t>c("Co-Spouse", "Other Relative", "Adopted/Foster Child", "Not Related", "Niece/Nephew By Blood", "Niece/Nephew By Marriage", "Son/Daughter", "Son/Daughter-in-law", "Grandchild", "Brother/Sister")</t>
+  </si>
+  <si>
+    <t>seq(7, 60)</t>
+  </si>
+  <si>
+    <t>seq(-600,600)</t>
+  </si>
+  <si>
+    <t>seq(-250000,250000)</t>
+  </si>
+  <si>
+    <t>seq(0, 40)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -884,8 +917,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Lucida Console"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1065,6 +1104,12 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -1242,12 +1287,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -1591,22 +1640,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K63"/>
+  <dimension ref="A1:K62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C51" sqref="C51"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B58" sqref="B58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.28515625" customWidth="1"/>
-    <col min="2" max="2" width="21.28515625" style="19" customWidth="1"/>
+    <col min="1" max="1" width="24.28515625" customWidth="1"/>
+    <col min="2" max="2" width="29" style="17" customWidth="1"/>
     <col min="3" max="3" width="32.85546875" customWidth="1"/>
     <col min="4" max="4" width="17.42578125" customWidth="1"/>
     <col min="5" max="5" width="15.140625" customWidth="1"/>
     <col min="6" max="6" width="13.42578125" customWidth="1"/>
-    <col min="7" max="8" width="13.42578125" style="19" customWidth="1"/>
+    <col min="7" max="8" width="13.42578125" style="17" customWidth="1"/>
     <col min="9" max="9" width="14.5703125" customWidth="1"/>
     <col min="10" max="10" width="31.5703125" customWidth="1"/>
   </cols>
@@ -1615,7 +1664,7 @@
       <c r="A1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="17" t="s">
         <v>187</v>
       </c>
       <c r="C1" t="s">
@@ -1630,10 +1679,10 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="19" t="s">
+      <c r="G1" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="H1" s="19" t="s">
+      <c r="H1" s="17" t="s">
         <v>190</v>
       </c>
       <c r="I1" t="s">
@@ -1646,1569 +1695,1576 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="B2" s="19"/>
-      <c r="E2" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="F2" s="3"/>
-      <c r="G2" s="19" t="s">
-        <v>198</v>
-      </c>
-      <c r="H2" s="18" t="s">
-        <v>194</v>
-      </c>
-      <c r="I2" s="19"/>
-    </row>
-    <row r="3" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="B3" s="19"/>
-      <c r="E3" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="F3" s="3"/>
-      <c r="G3" s="19" t="s">
-        <v>198</v>
-      </c>
-      <c r="H3" s="18" t="s">
-        <v>194</v>
-      </c>
-      <c r="I3" s="19"/>
+    <row r="2" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>200</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="G2" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="H2" s="17" t="s">
+        <v>191</v>
+      </c>
+      <c r="I2" s="17"/>
+      <c r="J2" s="11" t="str">
+        <f>CONCATENATE(A2, "=", E2, ",")</f>
+        <v>age=hc1,</v>
+      </c>
+      <c r="K2" s="11" t="str">
+        <f>CONCATENATE("table(pr$", A2, ")")</f>
+        <v>table(pr$age)</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>205</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="H3" s="17" t="s">
+        <v>191</v>
+      </c>
+      <c r="I3" s="17"/>
+      <c r="J3" s="11" t="str">
+        <f>CONCATENATE(A3, "=", E3, ",")</f>
+        <v>birth_order=hc64,</v>
+      </c>
+      <c r="K3" s="11" t="str">
+        <f>CONCATENATE("table(pr$", A3, ")")</f>
+        <v>table(pr$birth_order)</v>
+      </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>110</v>
-      </c>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="19" t="s">
-        <v>198</v>
-      </c>
-      <c r="I4" s="19"/>
+        <v>74</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>220</v>
+      </c>
+      <c r="D4" t="s">
+        <v>219</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="H4" s="17" t="s">
+        <v>191</v>
+      </c>
+      <c r="I4" s="17"/>
+      <c r="J4" t="str">
+        <f>CONCATENATE(A4, "=", F4, ",")</f>
+        <v>birth_weight=m19,</v>
+      </c>
+      <c r="K4" t="str">
+        <f>CONCATENATE("table(kr$", A4, ")")</f>
+        <v>table(kr$birth_weight)</v>
+      </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>111</v>
-      </c>
-      <c r="G5" s="19" t="s">
-        <v>198</v>
-      </c>
-      <c r="I5" s="19"/>
+        <v>98</v>
+      </c>
+      <c r="E5" t="s">
+        <v>133</v>
+      </c>
+      <c r="F5" t="s">
+        <v>186</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="H5" s="17" t="s">
+        <v>191</v>
+      </c>
+      <c r="I5" s="17"/>
+      <c r="J5" t="str">
+        <f>CONCATENATE(A5, "=", F5, ",")</f>
+        <v>birthday_cmc=b3,</v>
+      </c>
+      <c r="K5" t="str">
+        <f>CONCATENATE("table(kr$", A5, ")")</f>
+        <v>table(kr$birthday_cmc)</v>
+      </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>61</v>
-      </c>
-      <c r="B6" s="19" t="s">
-        <v>225</v>
-      </c>
-      <c r="C6" t="s">
-        <v>62</v>
+        <v>113</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>198</v>
       </c>
       <c r="E6" t="s">
         <v>133</v>
       </c>
-      <c r="F6" t="s">
-        <v>122</v>
-      </c>
-      <c r="G6" s="19" t="s">
+      <c r="F6" s="15" t="s">
+        <v>184</v>
+      </c>
+      <c r="G6" s="14" t="s">
         <v>175</v>
       </c>
-      <c r="H6" s="19" t="s">
-        <v>191</v>
-      </c>
-      <c r="I6" s="19"/>
-      <c r="J6" s="19" t="str">
+      <c r="H6" s="17" t="s">
+        <v>191</v>
+      </c>
+      <c r="I6" s="17"/>
+      <c r="J6" s="17" t="str">
         <f>CONCATENATE(A6, "=", F6, ",")</f>
-        <v>breastfeeding=derived from m4,</v>
-      </c>
-      <c r="K6" s="19" t="str">
-        <f t="shared" ref="K6:K17" si="0">CONCATENATE("table(kr$", A6, ")")</f>
-        <v>table(kr$breastfeeding)</v>
+        <v>birthmonth=b1,</v>
+      </c>
+      <c r="K6" s="17" t="str">
+        <f>CONCATENATE("table(kr$", A6, ")")</f>
+        <v>table(kr$birthmonth)</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>114</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>199</v>
+      </c>
+      <c r="E7" t="s">
+        <v>133</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>185</v>
+      </c>
+      <c r="G7" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="H7" s="17" t="s">
+        <v>191</v>
+      </c>
+      <c r="I7" s="17"/>
+      <c r="J7" s="17" t="str">
+        <f>CONCATENATE(A7, "=", F7, ",")</f>
+        <v>birthyear=b2,</v>
+      </c>
+      <c r="K7" s="17" t="str">
+        <f>CONCATENATE("table(kr$", A7, ")")</f>
+        <v>table(kr$birthyear)</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="B7" s="19" t="s">
-        <v>203</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="B8" s="17" t="s">
+        <v>200</v>
+      </c>
+      <c r="C8" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D8" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E8" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F8" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="G7" s="19" t="s">
+      <c r="G8" s="17" t="s">
         <v>175</v>
       </c>
-      <c r="H7" s="19" t="s">
-        <v>191</v>
-      </c>
-      <c r="I7" s="19"/>
-      <c r="J7" s="19" t="str">
-        <f t="shared" ref="J7:J18" si="1">CONCATENATE(A7, "=", F7, ",")</f>
+      <c r="H8" s="17" t="s">
+        <v>191</v>
+      </c>
+      <c r="J8" s="17" t="str">
+        <f>CONCATENATE(A8, "=", F8, ",")</f>
         <v>breast_duration=m4,</v>
       </c>
-      <c r="K7" s="19" t="str">
-        <f t="shared" si="0"/>
+      <c r="K8" s="17" t="str">
+        <f>CONCATENATE("table(kr$", A8, ")")</f>
         <v>table(kr$breast_duration)</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="19" t="s">
-        <v>74</v>
-      </c>
-      <c r="B8" s="19" t="s">
-        <v>227</v>
-      </c>
-      <c r="D8" s="19" t="s">
-        <v>226</v>
-      </c>
-      <c r="E8" s="19" t="s">
-        <v>75</v>
-      </c>
-      <c r="F8" s="19" t="s">
-        <v>75</v>
-      </c>
-      <c r="G8" s="16" t="s">
-        <v>175</v>
-      </c>
-      <c r="H8" s="19" t="s">
-        <v>191</v>
-      </c>
-      <c r="J8" s="19" t="str">
-        <f t="shared" si="1"/>
-        <v>birth_weight=m19,</v>
-      </c>
-      <c r="K8" s="19" t="str">
-        <f t="shared" si="0"/>
-        <v>table(kr$birth_weight)</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>163</v>
-      </c>
-      <c r="B9" s="19" t="s">
-        <v>225</v>
+        <v>61</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>218</v>
+      </c>
+      <c r="C9" t="s">
+        <v>62</v>
       </c>
       <c r="E9" t="s">
         <v>133</v>
       </c>
       <c r="F9" t="s">
-        <v>77</v>
-      </c>
-      <c r="G9" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="G9" s="17" t="s">
         <v>175</v>
       </c>
-      <c r="H9" s="19" t="s">
-        <v>191</v>
-      </c>
-      <c r="I9" s="19"/>
-      <c r="J9" s="19" t="str">
-        <f t="shared" si="1"/>
-        <v>istwin=b0,</v>
-      </c>
-      <c r="K9" s="19" t="str">
-        <f t="shared" si="0"/>
-        <v>table(kr$istwin)</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>178</v>
-      </c>
-      <c r="B10" s="19" t="s">
-        <v>228</v>
-      </c>
-      <c r="D10" t="s">
-        <v>12</v>
-      </c>
-      <c r="E10" t="s">
-        <v>180</v>
-      </c>
-      <c r="F10" t="s">
-        <v>181</v>
-      </c>
-      <c r="G10" s="16" t="s">
+      <c r="H9" s="17" t="s">
+        <v>191</v>
+      </c>
+      <c r="I9" s="17"/>
+      <c r="J9" s="17" t="str">
+        <f>CONCATENATE(A9, "=", F9, ",")</f>
+        <v>breastfeeding=derived from m4,</v>
+      </c>
+      <c r="K9" s="17" t="str">
+        <f>CONCATENATE("table(kr$", A9, ")")</f>
+        <v>table(kr$breastfeeding)</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="17" t="s">
+        <v>231</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>218</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>230</v>
+      </c>
+      <c r="F10" s="17" t="s">
+        <v>232</v>
+      </c>
+      <c r="G10" s="17" t="s">
         <v>175</v>
       </c>
-      <c r="H10" s="19" t="s">
-        <v>191</v>
-      </c>
-      <c r="I10" s="19"/>
-      <c r="J10" s="19" t="str">
-        <f t="shared" si="1"/>
-        <v>preceeding_interval=b11,</v>
-      </c>
-      <c r="K10" s="19" t="str">
-        <f t="shared" si="0"/>
-        <v>table(kr$preceeding_interval)</v>
+      <c r="H10" s="17" t="s">
+        <v>191</v>
+      </c>
+      <c r="K10" s="17" t="str">
+        <f>CONCATENATE("table(kr$", A10, ")")</f>
+        <v>table(kr$ever_breastfed)</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>179</v>
-      </c>
-      <c r="B11" s="19" t="s">
-        <v>228</v>
-      </c>
-      <c r="D11" t="s">
-        <v>12</v>
+        <v>171</v>
+      </c>
+      <c r="E11" t="s">
+        <v>173</v>
       </c>
       <c r="F11" t="s">
-        <v>182</v>
-      </c>
-      <c r="G11" s="16" t="s">
+        <v>172</v>
+      </c>
+      <c r="G11" s="17" t="s">
         <v>175</v>
       </c>
-      <c r="H11" s="19" t="s">
-        <v>191</v>
-      </c>
-      <c r="I11" s="19"/>
-      <c r="J11" s="19" t="str">
-        <f t="shared" si="1"/>
-        <v>suceeding_interval=b12,</v>
-      </c>
-      <c r="K11" s="19" t="str">
-        <f t="shared" si="0"/>
-        <v>table(kr$suceeding_interval)</v>
-      </c>
+      <c r="H11" s="16" t="s">
+        <v>192</v>
+      </c>
+      <c r="I11" s="17"/>
+      <c r="J11" s="17"/>
+      <c r="K11" s="17"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>82</v>
-      </c>
-      <c r="B12" s="19" t="s">
-        <v>225</v>
+        <v>33</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>133</v>
+        <v>34</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="G12" s="19" t="s">
-        <v>175</v>
-      </c>
-      <c r="H12" s="19" t="s">
-        <v>191</v>
-      </c>
-      <c r="I12" s="19"/>
-      <c r="J12" s="19" t="str">
-        <f t="shared" si="1"/>
-        <v>mother_smokes=v463z,</v>
-      </c>
-      <c r="K12" s="19" t="str">
-        <f t="shared" si="0"/>
-        <v>table(kr$mother_smokes)</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="G12" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="H12" s="16" t="s">
+        <v>192</v>
+      </c>
+      <c r="I12" s="17"/>
+      <c r="J12" s="17"/>
+      <c r="K12" s="17"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>86</v>
-      </c>
-      <c r="B13" s="19" t="s">
-        <v>229</v>
+        <v>226</v>
+      </c>
+      <c r="B13" s="17" t="s">
+        <v>233</v>
       </c>
       <c r="C13" t="s">
-        <v>87</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="G13" s="19" t="s">
-        <v>175</v>
-      </c>
-      <c r="H13" s="19" t="s">
-        <v>191</v>
-      </c>
-      <c r="I13" s="19"/>
-      <c r="J13" s="19" t="str">
-        <f t="shared" si="1"/>
-        <v>fever=h22,</v>
-      </c>
-      <c r="K13" s="19" t="str">
-        <f t="shared" si="0"/>
-        <v>table(kr$fever)</v>
-      </c>
+        <v>228</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="F13" s="3"/>
+      <c r="G13" s="17" t="s">
+        <v>177</v>
+      </c>
+      <c r="H13" s="17" t="s">
+        <v>191</v>
+      </c>
+      <c r="I13" s="17"/>
+      <c r="J13" s="17"/>
+      <c r="K13" s="17"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>113</v>
-      </c>
-      <c r="B14" s="19" t="s">
-        <v>200</v>
-      </c>
-      <c r="E14" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B14" s="17" t="s">
+        <v>218</v>
+      </c>
+      <c r="C14" t="s">
+        <v>101</v>
+      </c>
+      <c r="E14" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="F14" s="17" t="s">
-        <v>184</v>
-      </c>
-      <c r="G14" s="16" t="s">
+      <c r="F14" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="G14" s="17" t="s">
         <v>175</v>
       </c>
-      <c r="H14" s="19" t="s">
-        <v>191</v>
-      </c>
-      <c r="I14" s="19"/>
-      <c r="J14" s="19" t="str">
-        <f t="shared" si="1"/>
-        <v>birthmonth=b1,</v>
-      </c>
-      <c r="K14" s="19" t="str">
-        <f t="shared" si="0"/>
-        <v>table(kr$birthmonth)</v>
+      <c r="H14" s="17" t="s">
+        <v>191</v>
+      </c>
+      <c r="I14" s="17"/>
+      <c r="J14" s="17" t="str">
+        <f>CONCATENATE(A14, "=", F14, ",")</f>
+        <v>diarrhea=h11,</v>
+      </c>
+      <c r="K14" s="17" t="str">
+        <f>CONCATENATE("table(kr$", A14, ")")</f>
+        <v>table(kr$diarrhea)</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>114</v>
-      </c>
-      <c r="B15" s="19" t="s">
-        <v>201</v>
+        <v>212</v>
+      </c>
+      <c r="B15" s="17" t="s">
+        <v>243</v>
+      </c>
+      <c r="C15" t="s">
+        <v>215</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>133</v>
-      </c>
-      <c r="F15" s="17" t="s">
-        <v>185</v>
-      </c>
-      <c r="G15" s="16" t="s">
-        <v>175</v>
-      </c>
-      <c r="H15" s="19" t="s">
-        <v>191</v>
-      </c>
-      <c r="I15" s="19"/>
-      <c r="J15" s="19" t="str">
-        <f t="shared" si="1"/>
-        <v>birthyear=b2,</v>
-      </c>
-      <c r="K15" s="19" t="str">
-        <f t="shared" si="0"/>
-        <v>table(kr$birthyear)</v>
-      </c>
+        <v>138</v>
+      </c>
+      <c r="F15" s="8"/>
+      <c r="G15" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="H15" s="17" t="s">
+        <v>191</v>
+      </c>
+      <c r="I15" s="17"/>
+      <c r="J15" s="17" t="str">
+        <f>CONCATENATE(A15, "=", E15, ",")</f>
+        <v>drinkwatersource=hv201,</v>
+      </c>
+      <c r="K15" s="17"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>98</v>
+        <v>167</v>
+      </c>
+      <c r="B16" s="17" t="s">
+        <v>206</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>133</v>
-      </c>
-      <c r="F16" s="9" t="s">
-        <v>186</v>
-      </c>
-      <c r="G16" s="16" t="s">
-        <v>175</v>
-      </c>
-      <c r="H16" s="19" t="s">
-        <v>191</v>
-      </c>
-      <c r="I16" s="19"/>
-      <c r="J16" s="19" t="str">
-        <f t="shared" si="1"/>
-        <v>birthday_cmc=b3,</v>
-      </c>
-      <c r="K16" s="19" t="str">
-        <f t="shared" si="0"/>
-        <v>table(kr$birthday_cmc)</v>
+        <v>169</v>
+      </c>
+      <c r="F16" s="15"/>
+      <c r="G16" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="H16" s="17" t="s">
+        <v>191</v>
+      </c>
+      <c r="I16" s="17"/>
+      <c r="J16" s="17" t="str">
+        <f>CONCATENATE(A16, "=", E16, ",")</f>
+        <v>father_alive=hv113,</v>
+      </c>
+      <c r="K16" s="17" t="str">
+        <f>CONCATENATE("table(pr$", A16, ")")</f>
+        <v>table(pr$father_alive)</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>107</v>
-      </c>
-      <c r="B17" s="19" t="s">
-        <v>229</v>
-      </c>
-      <c r="D17" t="s">
-        <v>108</v>
+        <v>124</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>133</v>
-      </c>
-      <c r="F17" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="G17" s="16" t="s">
-        <v>175</v>
-      </c>
-      <c r="H17" s="19" t="s">
-        <v>191</v>
-      </c>
-      <c r="I17" s="19"/>
-      <c r="J17" s="19" t="str">
-        <f t="shared" si="1"/>
-        <v>parasite_drugs=h43,</v>
-      </c>
-      <c r="K17" s="19" t="str">
-        <f t="shared" si="0"/>
-        <v>table(kr$parasite_drugs)</v>
+        <v>170</v>
+      </c>
+      <c r="F17" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="G17" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="H17" s="17" t="s">
+        <v>192</v>
+      </c>
+      <c r="I17" s="17"/>
+      <c r="J17" t="str">
+        <f>CONCATENATE(A17, "=", E17, ",")</f>
+        <v>father_line=hv114,</v>
+      </c>
+      <c r="K17" t="str">
+        <f>CONCATENATE("table(pr$", A17, ")")</f>
+        <v>table(pr$father_line)</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>80</v>
-      </c>
-      <c r="B18" s="19" t="s">
-        <v>231</v>
-      </c>
-      <c r="C18" t="s">
-        <v>101</v>
-      </c>
-      <c r="E18" s="11" t="s">
-        <v>133</v>
-      </c>
-      <c r="F18" s="18" t="s">
-        <v>100</v>
-      </c>
-      <c r="G18" s="19" t="s">
-        <v>175</v>
-      </c>
-      <c r="H18" s="19" t="s">
-        <v>191</v>
-      </c>
-      <c r="I18" s="19"/>
-      <c r="J18" s="19" t="str">
-        <f t="shared" si="1"/>
-        <v>diarrhea=h11,</v>
-      </c>
-      <c r="K18" s="19" t="str">
-        <f>CONCATENATE("table(kr$", A18, ")")</f>
-        <v>table(kr$diarrhea)</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>195</v>
-      </c>
-      <c r="B19" s="19" t="s">
-        <v>200</v>
-      </c>
-      <c r="E19" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="F19" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="G19" s="19" t="s">
-        <v>139</v>
-      </c>
-      <c r="H19" s="19" t="s">
-        <v>191</v>
-      </c>
-      <c r="I19" s="19"/>
-      <c r="J19" t="str">
-        <f>CONCATENATE(A19, "=", E19, ",")</f>
-        <v>interview_month=hv006,</v>
-      </c>
-      <c r="K19" t="str">
-        <f>CONCATENATE("table(pr$", A19, ")")</f>
-        <v>table(pr$interview_month)</v>
+        <v>189</v>
+      </c>
+      <c r="B18" s="17" t="s">
+        <v>235</v>
+      </c>
+      <c r="D18" t="s">
+        <v>211</v>
+      </c>
+      <c r="E18" t="s">
+        <v>223</v>
+      </c>
+      <c r="G18" s="17" t="s">
+        <v>177</v>
+      </c>
+      <c r="H18" s="17" t="s">
+        <v>191</v>
+      </c>
+      <c r="I18" s="17"/>
+      <c r="J18" s="17"/>
+      <c r="K18" s="17"/>
+    </row>
+    <row r="19" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="17" t="s">
+        <v>234</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>236</v>
+      </c>
+      <c r="E19" s="17" t="s">
+        <v>160</v>
+      </c>
+      <c r="G19" s="14" t="s">
+        <v>177</v>
+      </c>
+      <c r="H19" s="17" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>196</v>
-      </c>
-      <c r="B20" s="19" t="s">
-        <v>201</v>
+        <v>86</v>
+      </c>
+      <c r="B20" s="17" t="s">
+        <v>218</v>
+      </c>
+      <c r="C20" t="s">
+        <v>87</v>
       </c>
       <c r="E20" t="s">
-        <v>41</v>
+        <v>133</v>
       </c>
       <c r="F20" t="s">
-        <v>42</v>
-      </c>
-      <c r="G20" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="G20" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="H20" s="17" t="s">
+        <v>191</v>
+      </c>
+      <c r="I20" s="17"/>
+      <c r="J20" s="17" t="str">
+        <f>CONCATENATE(A20, "=", F20, ",")</f>
+        <v>fever=h22,</v>
+      </c>
+      <c r="K20" s="17" t="str">
+        <f>CONCATENATE("table(kr$", A20, ")")</f>
+        <v>table(kr$fever)</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21" s="17" t="s">
+        <v>246</v>
+      </c>
+      <c r="D21" t="s">
+        <v>203</v>
+      </c>
+      <c r="E21" t="s">
+        <v>23</v>
+      </c>
+      <c r="F21" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="G21" s="17" t="s">
         <v>139</v>
       </c>
-      <c r="H20" s="19" t="s">
-        <v>191</v>
-      </c>
-      <c r="I20" s="19"/>
-      <c r="J20" s="19" t="str">
-        <f t="shared" ref="J20:J49" si="2">CONCATENATE(A20, "=", E20, ",")</f>
-        <v>interview_year=hv007,</v>
-      </c>
-      <c r="K20" s="19" t="str">
-        <f t="shared" ref="K20:K49" si="3">CONCATENATE("table(pr$", A20, ")")</f>
-        <v>table(pr$interview_year)</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="19" t="s">
-        <v>97</v>
-      </c>
-      <c r="B21" s="19" t="s">
-        <v>202</v>
-      </c>
-      <c r="E21" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="F21" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="G21" s="19" t="s">
-        <v>139</v>
-      </c>
-      <c r="H21" s="18" t="s">
-        <v>191</v>
-      </c>
-      <c r="J21" s="19" t="str">
-        <f t="shared" si="2"/>
-        <v>interview_cmc=hv008,</v>
-      </c>
-      <c r="K21" s="19" t="str">
-        <f t="shared" si="3"/>
-        <v>table(pr$interview_cmc)</v>
+      <c r="H21" s="17" t="s">
+        <v>191</v>
+      </c>
+      <c r="I21" s="17"/>
+      <c r="J21" s="17" t="str">
+        <f>CONCATENATE(A21, "=", E21, ",")</f>
+        <v>haz_dhs=hc5,</v>
+      </c>
+      <c r="K21" s="17" t="str">
+        <f>CONCATENATE("table(pr$", A21, ")")</f>
+        <v>table(pr$haz_dhs)</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>0</v>
-      </c>
-      <c r="B22" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22" s="17" t="s">
+        <v>246</v>
+      </c>
+      <c r="D22" t="s">
         <v>203</v>
       </c>
-      <c r="D22" t="s">
-        <v>12</v>
-      </c>
       <c r="E22" t="s">
-        <v>129</v>
+        <v>53</v>
       </c>
       <c r="F22" t="s">
-        <v>117</v>
-      </c>
-      <c r="G22" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="G22" s="17" t="s">
         <v>139</v>
       </c>
-      <c r="H22" s="19" t="s">
-        <v>191</v>
-      </c>
-      <c r="I22" s="19"/>
-      <c r="J22" s="19" t="str">
-        <f t="shared" si="2"/>
-        <v>age=hc1,</v>
-      </c>
-      <c r="K22" s="19" t="str">
-        <f t="shared" si="3"/>
-        <v>table(pr$age)</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="H22" s="17" t="s">
+        <v>191</v>
+      </c>
+      <c r="I22" s="17"/>
+      <c r="J22" s="17" t="str">
+        <f>CONCATENATE(A22, "=", E22, ",")</f>
+        <v>haz_who=hc70,</v>
+      </c>
+      <c r="K22" s="17" t="str">
+        <f>CONCATENATE("table(pr$", A22, ")")</f>
+        <v>table(pr$haz_who)</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="B23" s="17" t="s">
+        <v>210</v>
+      </c>
+      <c r="D23" s="17" t="s">
+        <v>211</v>
+      </c>
+      <c r="E23" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="F23" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="G23" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="H23" s="16" t="s">
+        <v>191</v>
+      </c>
+      <c r="J23" s="17" t="str">
+        <f>CONCATENATE(A23, "=", E23, ",")</f>
+        <v>head_age=hv220,</v>
+      </c>
+      <c r="K23" s="17" t="str">
+        <f>CONCATENATE("table(pr$", A23, ")")</f>
+        <v>table(pr$head_age)</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="B24" s="17" t="s">
+        <v>204</v>
+      </c>
+      <c r="E24" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="F24" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="G24" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="H24" s="16" t="s">
+        <v>191</v>
+      </c>
+      <c r="J24" s="17" t="str">
+        <f>CONCATENATE(A24, "=", E24, ",")</f>
+        <v>head_sex=hv219,</v>
+      </c>
+      <c r="K24" s="17" t="str">
+        <f>CONCATENATE("table(pr$", A24, ")")</f>
+        <v>table(pr$head_sex)</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B23" s="19" t="s">
-        <v>204</v>
-      </c>
-      <c r="D23" t="s">
+      <c r="B25" s="17" t="s">
+        <v>237</v>
+      </c>
+      <c r="D25" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E25" s="17" t="s">
         <v>130</v>
       </c>
-      <c r="F23" s="14" t="s">
+      <c r="F25" s="17" t="s">
         <v>119</v>
       </c>
-      <c r="G23" s="19" t="s">
+      <c r="G25" s="17" t="s">
         <v>139</v>
       </c>
-      <c r="H23" s="19" t="s">
-        <v>191</v>
-      </c>
-      <c r="I23" s="19"/>
-      <c r="J23" s="19" t="str">
-        <f t="shared" si="2"/>
+      <c r="H25" s="17" t="s">
+        <v>191</v>
+      </c>
+      <c r="J25" s="17" t="str">
+        <f>CONCATENATE(A25, "=", E25, ",")</f>
         <v>height=hc3,</v>
       </c>
-      <c r="K23" s="19" t="str">
-        <f t="shared" si="3"/>
+      <c r="K25" s="17" t="str">
+        <f>CONCATENATE("table(pr$", A25, ")")</f>
         <v>table(pr$height)</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>6</v>
-      </c>
-      <c r="B24" s="19" t="s">
-        <v>205</v>
-      </c>
-      <c r="D24" t="s">
-        <v>10</v>
-      </c>
-      <c r="E24" t="s">
-        <v>131</v>
-      </c>
-      <c r="F24" t="s">
-        <v>118</v>
-      </c>
-      <c r="G24" s="19" t="s">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>91</v>
+      </c>
+      <c r="B26" s="17" t="s">
+        <v>239</v>
+      </c>
+      <c r="D26" s="17"/>
+      <c r="E26" t="s">
+        <v>91</v>
+      </c>
+      <c r="H26" s="17" t="s">
+        <v>192</v>
+      </c>
+      <c r="I26" s="17"/>
+      <c r="J26" s="17"/>
+      <c r="K26" s="17"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>45</v>
+      </c>
+      <c r="B27" s="14" t="s">
+        <v>238</v>
+      </c>
+      <c r="D27" s="17"/>
+      <c r="E27" t="s">
+        <v>135</v>
+      </c>
+      <c r="G27" s="17" t="s">
         <v>139</v>
       </c>
-      <c r="H24" s="19" t="s">
-        <v>191</v>
-      </c>
-      <c r="I24" s="19"/>
-      <c r="J24" s="19" t="str">
-        <f t="shared" si="2"/>
-        <v>weight=hc2,</v>
-      </c>
-      <c r="K24" s="19" t="str">
-        <f t="shared" si="3"/>
-        <v>table(pr$weight)</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="19" t="s">
-        <v>162</v>
-      </c>
-      <c r="B25" s="19" t="s">
-        <v>206</v>
-      </c>
-      <c r="E25" s="19" t="s">
-        <v>144</v>
-      </c>
-      <c r="F25" s="19" t="s">
-        <v>176</v>
-      </c>
-      <c r="G25" s="19" t="s">
-        <v>139</v>
-      </c>
-      <c r="H25" s="19" t="s">
-        <v>191</v>
-      </c>
-      <c r="J25" s="19" t="str">
-        <f t="shared" si="2"/>
-        <v>how_measured=hc15,</v>
-      </c>
-      <c r="K25" s="19" t="str">
-        <f t="shared" si="3"/>
-        <v>table(pr$how_measured)</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="B26" s="19" t="str">
-        <f>"-600 &lt; x &lt; 600"</f>
-        <v>-600 &lt; x &lt; 600</v>
-      </c>
-      <c r="D26" s="19" t="s">
-        <v>207</v>
-      </c>
-      <c r="E26" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="F26" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="G26" s="19" t="s">
-        <v>139</v>
-      </c>
-      <c r="H26" s="19" t="s">
-        <v>191</v>
-      </c>
-      <c r="J26" s="19" t="str">
-        <f t="shared" si="2"/>
-        <v>haz_dhs=hc5,</v>
-      </c>
-      <c r="K26" s="19" t="str">
-        <f t="shared" si="3"/>
-        <v>table(pr$haz_dhs)</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="B27" s="19" t="str">
-        <f t="shared" ref="B27:B31" si="4">"-600 &lt; x &lt; 600"</f>
-        <v>-600 &lt; x &lt; 600</v>
-      </c>
-      <c r="D27" s="19" t="s">
-        <v>207</v>
-      </c>
-      <c r="E27" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="F27" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="G27" s="19" t="s">
-        <v>139</v>
-      </c>
-      <c r="H27" s="19" t="s">
-        <v>191</v>
-      </c>
-      <c r="J27" s="19" t="str">
-        <f t="shared" si="2"/>
-        <v>whz_dhs=hc11,</v>
-      </c>
-      <c r="K27" s="19" t="str">
-        <f t="shared" si="3"/>
-        <v>table(pr$whz_dhs)</v>
+      <c r="H27" s="17" t="s">
+        <v>191</v>
+      </c>
+      <c r="I27" s="17"/>
+      <c r="J27" s="17" t="str">
+        <f>CONCATENATE(A27, "=", E27, ",")</f>
+        <v>hhsize=hv009,</v>
+      </c>
+      <c r="K27" s="17" t="str">
+        <f>CONCATENATE("table(pr$", A27, ")")</f>
+        <v>table(pr$hhsize)</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>19</v>
-      </c>
-      <c r="B28" s="19" t="str">
-        <f t="shared" si="4"/>
-        <v>-600 &lt; x &lt; 600</v>
-      </c>
-      <c r="D28" s="19" t="s">
-        <v>207</v>
-      </c>
+        <v>162</v>
+      </c>
+      <c r="B28" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="D28" s="17"/>
       <c r="E28" t="s">
-        <v>25</v>
+        <v>144</v>
       </c>
       <c r="F28" t="s">
-        <v>26</v>
-      </c>
-      <c r="G28" s="19" t="s">
+        <v>176</v>
+      </c>
+      <c r="G28" s="17" t="s">
         <v>139</v>
       </c>
-      <c r="H28" s="19" t="s">
-        <v>191</v>
-      </c>
-      <c r="I28" s="19"/>
-      <c r="J28" s="19" t="str">
-        <f t="shared" si="2"/>
-        <v>waz_dhs=hc8,</v>
-      </c>
-      <c r="K28" s="19" t="str">
-        <f t="shared" si="3"/>
-        <v>table(pr$waz_dhs)</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>20</v>
-      </c>
-      <c r="B29" s="19" t="str">
-        <f t="shared" si="4"/>
-        <v>-600 &lt; x &lt; 600</v>
-      </c>
-      <c r="D29" s="19" t="s">
-        <v>207</v>
-      </c>
-      <c r="E29" t="s">
-        <v>53</v>
-      </c>
-      <c r="F29" t="s">
-        <v>54</v>
-      </c>
-      <c r="G29" s="19" t="s">
+      <c r="H28" s="17" t="s">
+        <v>191</v>
+      </c>
+      <c r="I28" s="17"/>
+      <c r="J28" s="17" t="str">
+        <f>CONCATENATE(A28, "=", E28, ",")</f>
+        <v>how_measured=hc15,</v>
+      </c>
+      <c r="K28" s="17" t="str">
+        <f>CONCATENATE("table(pr$", A28, ")")</f>
+        <v>table(pr$how_measured)</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="B29" s="17"/>
+      <c r="D29" s="17"/>
+      <c r="E29" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="F29" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="G29" s="17" t="s">
         <v>139</v>
       </c>
-      <c r="H29" s="19" t="s">
-        <v>191</v>
-      </c>
-      <c r="I29" s="19"/>
-      <c r="J29" s="19" t="str">
-        <f t="shared" si="2"/>
-        <v>haz_who=hc70,</v>
-      </c>
-      <c r="K29" s="19" t="str">
-        <f t="shared" si="3"/>
-        <v>table(pr$haz_who)</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>21</v>
-      </c>
-      <c r="B30" s="19" t="str">
-        <f t="shared" si="4"/>
-        <v>-600 &lt; x &lt; 600</v>
-      </c>
-      <c r="D30" s="19" t="s">
-        <v>207</v>
-      </c>
-      <c r="E30" t="s">
-        <v>55</v>
-      </c>
-      <c r="F30" t="s">
-        <v>56</v>
-      </c>
-      <c r="G30" s="19" t="s">
+      <c r="H29" s="16" t="s">
+        <v>191</v>
+      </c>
+      <c r="I29" s="17"/>
+      <c r="J29" s="17" t="str">
+        <f>CONCATENATE(A29, "=", E29, ",")</f>
+        <v>interview_cmc=hv008,</v>
+      </c>
+      <c r="K29" s="17" t="str">
+        <f>CONCATENATE("table(pr$", A29, ")")</f>
+        <v>table(pr$interview_cmc)</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="B30" s="17" t="s">
+        <v>198</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F30" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="G30" s="17" t="s">
         <v>139</v>
       </c>
-      <c r="H30" s="19" t="s">
-        <v>191</v>
-      </c>
-      <c r="I30" s="19"/>
-      <c r="J30" s="19" t="str">
-        <f t="shared" si="2"/>
-        <v>whz_who=hc72,</v>
-      </c>
-      <c r="K30" s="19" t="str">
-        <f t="shared" si="3"/>
-        <v>table(pr$whz_who)</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="B31" s="19" t="str">
-        <f t="shared" si="4"/>
-        <v>-600 &lt; x &lt; 600</v>
-      </c>
-      <c r="D31" s="19" t="s">
-        <v>207</v>
-      </c>
-      <c r="E31" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="F31" s="19" t="s">
-        <v>58</v>
-      </c>
-      <c r="G31" s="19" t="s">
+      <c r="H30" s="17" t="s">
+        <v>191</v>
+      </c>
+      <c r="I30" s="17"/>
+      <c r="J30" s="17" t="str">
+        <f>CONCATENATE(A30, "=", E30, ",")</f>
+        <v>interview_month=hv006,</v>
+      </c>
+      <c r="K30" s="17" t="str">
+        <f>CONCATENATE("table(pr$", A30, ")")</f>
+        <v>table(pr$interview_month)</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="B31" s="17" t="s">
+        <v>199</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F31" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="G31" s="17" t="s">
         <v>139</v>
       </c>
-      <c r="H31" s="19" t="s">
-        <v>191</v>
-      </c>
-      <c r="I31" s="19"/>
-      <c r="J31" s="19" t="str">
-        <f t="shared" si="2"/>
-        <v>waz_who=hc71,</v>
-      </c>
-      <c r="K31" s="19" t="str">
-        <f t="shared" si="3"/>
-        <v>table(pr$waz_who)</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="B32" s="19" t="s">
-        <v>208</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="F32" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="G32" s="19" t="s">
+      <c r="H31" s="17" t="s">
+        <v>191</v>
+      </c>
+      <c r="I31" s="17"/>
+      <c r="J31" s="17" t="str">
+        <f>CONCATENATE(A31, "=", E31, ",")</f>
+        <v>interview_year=hv007,</v>
+      </c>
+      <c r="K31" s="17" t="str">
+        <f>CONCATENATE("table(pr$", A31, ")")</f>
+        <v>table(pr$interview_year)</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="B32" s="17" t="s">
+        <v>218</v>
+      </c>
+      <c r="E32" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="F32" t="s">
+        <v>77</v>
+      </c>
+      <c r="G32" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="H32" s="17" t="s">
+        <v>191</v>
+      </c>
+      <c r="I32" s="17"/>
+      <c r="J32" s="17" t="str">
+        <f>CONCATENATE(A32, "=", F32, ",")</f>
+        <v>istwin=b0,</v>
+      </c>
+      <c r="K32" s="17" t="str">
+        <f>CONCATENATE("table(kr$", A32, ")")</f>
+        <v>table(kr$istwin)</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="G33" s="17" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B34" s="17"/>
+      <c r="F34" s="17"/>
+      <c r="G34" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="H34" s="17"/>
+      <c r="I34" s="17"/>
+      <c r="J34" s="17"/>
+      <c r="K34" s="17"/>
+    </row>
+    <row r="35" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="17" t="s">
+        <v>166</v>
+      </c>
+      <c r="B35" s="17" t="s">
+        <v>218</v>
+      </c>
+      <c r="E35" s="17" t="s">
+        <v>168</v>
+      </c>
+      <c r="G35" s="14" t="s">
         <v>139</v>
       </c>
-      <c r="H32" s="19" t="s">
-        <v>191</v>
-      </c>
-      <c r="I32" s="19"/>
-      <c r="J32" s="19" t="str">
-        <f t="shared" si="2"/>
-        <v>sex=hc27,</v>
-      </c>
-      <c r="K32" s="19" t="str">
-        <f t="shared" si="3"/>
-        <v>table(pr$sex)</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="B33" s="16" t="s">
-        <v>209</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="F33" s="19"/>
-      <c r="G33" s="19" t="s">
+      <c r="H35" s="17" t="s">
+        <v>191</v>
+      </c>
+      <c r="J35" s="17" t="str">
+        <f>CONCATENATE(A35, "=", E35, ",")</f>
+        <v>mother_alive=hv111,</v>
+      </c>
+      <c r="K35" s="17" t="str">
+        <f>CONCATENATE("table(pr$", A35, ")")</f>
+        <v>table(pr$mother_alive)</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B36" s="17"/>
+      <c r="E36" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="F36" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="G36" s="14" t="s">
         <v>139</v>
       </c>
-      <c r="H33" s="19" t="s">
-        <v>191</v>
-      </c>
-      <c r="I33" s="19"/>
-      <c r="J33" s="19" t="str">
-        <f t="shared" si="2"/>
-        <v>relationship_hhhead=hv101,</v>
-      </c>
-      <c r="K33" s="19" t="str">
-        <f t="shared" si="3"/>
-        <v>table(pr$relationship_hhhead)</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="B34" s="19" t="s">
-        <v>210</v>
-      </c>
-      <c r="E34" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="F34" t="s">
-        <v>73</v>
-      </c>
-      <c r="G34" s="16" t="s">
-        <v>139</v>
-      </c>
-      <c r="H34" s="19" t="s">
-        <v>191</v>
-      </c>
-      <c r="I34" s="19"/>
-      <c r="J34" s="19" t="str">
-        <f t="shared" si="2"/>
-        <v>birth_order=hc64,</v>
-      </c>
-      <c r="K34" s="19" t="str">
-        <f t="shared" si="3"/>
-        <v>table(pr$birth_order)</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="19" t="s">
-        <v>166</v>
-      </c>
-      <c r="B35" s="19" t="s">
+      <c r="H36" s="17" t="s">
+        <v>192</v>
+      </c>
+      <c r="I36" s="17"/>
+      <c r="J36" s="17" t="str">
+        <f>CONCATENATE(A36, "=", E36, ",")</f>
+        <v>mother_line=hv112,</v>
+      </c>
+      <c r="K36" s="17" t="str">
+        <f>CONCATENATE("table(pr$", A36, ")")</f>
+        <v>table(pr$mother_line)</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>82</v>
+      </c>
+      <c r="B37" s="17" t="s">
+        <v>218</v>
+      </c>
+      <c r="E37" t="s">
+        <v>133</v>
+      </c>
+      <c r="F37" t="s">
+        <v>183</v>
+      </c>
+      <c r="G37" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="H37" s="17" t="s">
+        <v>191</v>
+      </c>
+      <c r="I37" s="17"/>
+      <c r="J37" s="17" t="str">
+        <f>CONCATENATE(A37, "=", F37, ",")</f>
+        <v>mother_smokes=v463z,</v>
+      </c>
+      <c r="K37" s="17" t="str">
+        <f>CONCATENATE("table(kr$", A37, ")")</f>
+        <v>table(kr$mother_smokes)</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>188</v>
+      </c>
+      <c r="B38" s="17" t="s">
+        <v>240</v>
+      </c>
+      <c r="D38" t="s">
         <v>211</v>
       </c>
-      <c r="E35" s="19" t="s">
-        <v>168</v>
-      </c>
-      <c r="G35" s="16" t="s">
-        <v>139</v>
-      </c>
-      <c r="H35" s="19" t="s">
-        <v>191</v>
-      </c>
-      <c r="J35" s="19" t="str">
-        <f t="shared" si="2"/>
-        <v>mother_alive=hv111,</v>
-      </c>
-      <c r="K35" s="19" t="str">
-        <f t="shared" si="3"/>
-        <v>table(pr$mother_alive)</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="B36" s="19"/>
-      <c r="E36" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="F36" s="17" t="s">
-        <v>94</v>
-      </c>
-      <c r="G36" s="16" t="s">
-        <v>139</v>
-      </c>
-      <c r="H36" s="19" t="s">
-        <v>192</v>
-      </c>
-      <c r="I36" s="19"/>
-      <c r="J36" s="19" t="str">
-        <f t="shared" si="2"/>
-        <v>mother_line=hv112,</v>
-      </c>
-      <c r="K36" s="19" t="str">
-        <f t="shared" si="3"/>
-        <v>table(pr$mother_line)</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="19" t="s">
-        <v>167</v>
-      </c>
-      <c r="B37" s="19" t="s">
-        <v>211</v>
-      </c>
-      <c r="E37" s="19" t="s">
-        <v>169</v>
-      </c>
-      <c r="F37" s="17"/>
-      <c r="G37" s="16" t="s">
-        <v>139</v>
-      </c>
-      <c r="H37" s="19" t="s">
-        <v>191</v>
-      </c>
-      <c r="J37" s="19" t="str">
-        <f t="shared" si="2"/>
-        <v>father_alive=hv113,</v>
-      </c>
-      <c r="K37" s="19" t="str">
-        <f t="shared" si="3"/>
-        <v>table(pr$father_alive)</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="B38" s="19"/>
-      <c r="E38" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="F38" s="17" t="s">
-        <v>128</v>
-      </c>
-      <c r="G38" s="16" t="s">
-        <v>139</v>
-      </c>
-      <c r="H38" s="19" t="s">
-        <v>192</v>
-      </c>
-      <c r="I38" s="19"/>
-      <c r="J38" s="19" t="str">
-        <f t="shared" si="2"/>
-        <v>father_line=hv114,</v>
-      </c>
-      <c r="K38" s="19" t="str">
-        <f t="shared" si="3"/>
-        <v>table(pr$father_line)</v>
-      </c>
+      <c r="E38" t="s">
+        <v>223</v>
+      </c>
+      <c r="G38" s="17" t="s">
+        <v>177</v>
+      </c>
+      <c r="H38" s="17" t="s">
+        <v>191</v>
+      </c>
+      <c r="I38" s="17"/>
+      <c r="J38" s="17"/>
+      <c r="K38" s="17"/>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>45</v>
-      </c>
-      <c r="B39" s="19" t="s">
-        <v>212</v>
-      </c>
-      <c r="E39" t="s">
-        <v>135</v>
-      </c>
-      <c r="G39" s="19" t="s">
-        <v>139</v>
-      </c>
-      <c r="H39" s="19" t="s">
-        <v>191</v>
-      </c>
-      <c r="I39" s="19"/>
-      <c r="J39" s="19" t="str">
-        <f t="shared" si="2"/>
-        <v>hhsize=hv009,</v>
-      </c>
-      <c r="K39" s="19" t="str">
-        <f t="shared" si="3"/>
-        <v>table(pr$hhsize)</v>
-      </c>
+        <v>241</v>
+      </c>
+      <c r="B39" s="17" t="s">
+        <v>242</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="F39" s="5"/>
+      <c r="G39" s="17" t="s">
+        <v>177</v>
+      </c>
+      <c r="H39" s="17" t="s">
+        <v>191</v>
+      </c>
+      <c r="I39" s="17"/>
+      <c r="J39" s="17"/>
+      <c r="K39" s="17"/>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>47</v>
-      </c>
-      <c r="B40" s="19" t="s">
         <v>213</v>
       </c>
+      <c r="B40" s="17" t="s">
+        <v>243</v>
+      </c>
+      <c r="C40" t="s">
+        <v>216</v>
+      </c>
       <c r="E40" t="s">
-        <v>48</v>
+        <v>214</v>
       </c>
       <c r="F40" t="s">
-        <v>120</v>
-      </c>
-      <c r="G40" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="G40" s="17" t="s">
         <v>139</v>
       </c>
-      <c r="H40" s="19" t="s">
-        <v>191</v>
-      </c>
-      <c r="I40" s="19"/>
-      <c r="J40" s="19" t="str">
-        <f t="shared" si="2"/>
-        <v>urban_rural=hv025,</v>
-      </c>
-      <c r="K40" s="19" t="str">
-        <f t="shared" si="3"/>
-        <v>table(pr$urban_rural)</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>49</v>
-      </c>
-      <c r="B41" s="19" t="s">
-        <v>214</v>
-      </c>
-      <c r="E41" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="F41" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="G41" s="19" t="s">
-        <v>139</v>
-      </c>
-      <c r="H41" s="19" t="s">
-        <v>191</v>
-      </c>
-      <c r="I41" s="19"/>
-      <c r="J41" s="19" t="str">
-        <f t="shared" si="2"/>
-        <v>wealth_index=hv270,</v>
-      </c>
-      <c r="K41" s="19" t="str">
-        <f t="shared" si="3"/>
-        <v>table(pr$wealth_index)</v>
+      <c r="H40" s="17" t="s">
+        <v>191</v>
+      </c>
+      <c r="I40" s="17"/>
+      <c r="J40" s="17" t="str">
+        <f>CONCATENATE(A40, "=", E40, ",")</f>
+        <v>otherwatersource=hv202,</v>
+      </c>
+      <c r="K40" s="17" t="str">
+        <f>CONCATENATE("table(pr$", A40, ")")</f>
+        <v>table(pr$otherwatersource)</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="B41" s="17" t="s">
+        <v>222</v>
+      </c>
+      <c r="D41" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="E41" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="F41" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="G41" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="H41" s="17" t="s">
+        <v>191</v>
+      </c>
+      <c r="J41" s="17" t="str">
+        <f>CONCATENATE(A41, "=", F41, ",")</f>
+        <v>parasite_drugs=h43,</v>
+      </c>
+      <c r="K41" s="17" t="str">
+        <f>CONCATENATE("table(kr$", A41, ")")</f>
+        <v>table(kr$parasite_drugs)</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>50</v>
-      </c>
-      <c r="B42" s="19" t="str">
-        <f>"-250000 &lt; x &lt; 250000"</f>
-        <v>-250000 &lt; x &lt; 250000</v>
-      </c>
-      <c r="E42" t="s">
-        <v>137</v>
-      </c>
-      <c r="F42" t="s">
-        <v>52</v>
-      </c>
-      <c r="G42" s="19" t="s">
+        <v>178</v>
+      </c>
+      <c r="B42" s="17" t="s">
+        <v>221</v>
+      </c>
+      <c r="D42" t="s">
+        <v>12</v>
+      </c>
+      <c r="E42" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="F42" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="G42" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="H42" s="17" t="s">
+        <v>191</v>
+      </c>
+      <c r="I42" s="17"/>
+      <c r="J42" s="17" t="str">
+        <f>CONCATENATE(A42, "=", F42, ",")</f>
+        <v>preceeding_interval=b11,</v>
+      </c>
+      <c r="K42" s="17" t="str">
+        <f>CONCATENATE("table(kr$", A42, ")")</f>
+        <v>table(kr$preceeding_interval)</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>197</v>
+      </c>
+      <c r="B43" s="14" t="s">
+        <v>244</v>
+      </c>
+      <c r="E43" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="F43" s="17"/>
+      <c r="G43" s="17" t="s">
         <v>139</v>
       </c>
-      <c r="H42" s="19" t="s">
-        <v>191</v>
-      </c>
-      <c r="I42" s="19"/>
-      <c r="J42" s="19" t="str">
-        <f t="shared" si="2"/>
-        <v>wealth_factor=hv271,</v>
-      </c>
-      <c r="K42" s="19" t="str">
-        <f t="shared" si="3"/>
-        <v>table(pr$wealth_factor)</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="19" t="s">
-        <v>218</v>
-      </c>
-      <c r="B43" s="19" t="s">
-        <v>221</v>
-      </c>
-      <c r="C43" s="19" t="s">
-        <v>222</v>
-      </c>
-      <c r="E43" s="19" t="s">
-        <v>138</v>
-      </c>
-      <c r="G43" s="19" t="s">
-        <v>139</v>
-      </c>
-      <c r="H43" s="19" t="s">
-        <v>191</v>
-      </c>
-      <c r="J43" s="19" t="str">
-        <f t="shared" si="2"/>
-        <v>drinkwatersource=hv201,</v>
+      <c r="H43" s="17" t="s">
+        <v>191</v>
+      </c>
+      <c r="I43" s="17"/>
+      <c r="J43" s="17" t="str">
+        <f>CONCATENATE(A43, "=", E43, ",")</f>
+        <v>relationship_hhhead=hv101,</v>
+      </c>
+      <c r="K43" s="17" t="str">
+        <f>CONCATENATE("table(pr$", A43, ")")</f>
+        <v>table(pr$relationship_hhhead)</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>219</v>
-      </c>
-      <c r="B44" s="19" t="s">
-        <v>221</v>
-      </c>
-      <c r="C44" t="s">
-        <v>223</v>
-      </c>
-      <c r="E44" s="7" t="s">
-        <v>220</v>
-      </c>
-      <c r="F44" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="G44" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="E44" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="F44" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="G44" s="16" t="s">
         <v>139</v>
       </c>
-      <c r="H44" s="19" t="s">
-        <v>191</v>
-      </c>
-      <c r="I44" s="19"/>
-      <c r="J44" s="19" t="str">
-        <f t="shared" si="2"/>
-        <v>otherwatersource=hv202,</v>
-      </c>
-      <c r="K44" s="19" t="str">
-        <f t="shared" si="3"/>
-        <v>table(pr$otherwatersource)</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>102</v>
-      </c>
-      <c r="B45" s="19" t="s">
-        <v>215</v>
-      </c>
-      <c r="C45" t="s">
-        <v>224</v>
-      </c>
-      <c r="D45" t="s">
-        <v>103</v>
-      </c>
-      <c r="E45" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="F45" s="18" t="s">
-        <v>104</v>
-      </c>
-      <c r="G45" s="19" t="s">
+      <c r="H44" s="16" t="s">
+        <v>191</v>
+      </c>
+      <c r="I44" s="17"/>
+      <c r="J44" s="17" t="str">
+        <f>CONCATENATE(A44, "=", E44, ",")</f>
+        <v>sampweight=hv005,</v>
+      </c>
+      <c r="K44" s="17" t="str">
+        <f>CONCATENATE("table(pr$", A44, ")")</f>
+        <v>table(pr$sampweight)</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="B45" s="17" t="s">
+        <v>204</v>
+      </c>
+      <c r="E45" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="F45" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="G45" s="17" t="s">
         <v>139</v>
       </c>
-      <c r="H45" s="19" t="s">
-        <v>191</v>
-      </c>
-      <c r="I45" s="19"/>
-      <c r="J45" s="19" t="str">
-        <f t="shared" si="2"/>
-        <v>watersource_dist=hv204,</v>
-      </c>
-      <c r="K45" s="19" t="str">
-        <f t="shared" si="3"/>
-        <v>table(pr$watersource_dist)</v>
+      <c r="H45" s="17" t="s">
+        <v>191</v>
+      </c>
+      <c r="I45" s="17"/>
+      <c r="J45" s="17" t="str">
+        <f>CONCATENATE(A45, "=", E45, ",")</f>
+        <v>sex=hc27,</v>
+      </c>
+      <c r="K45" s="17" t="str">
+        <f>CONCATENATE("table(pr$", A45, ")")</f>
+        <v>table(pr$sex)</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>84</v>
-      </c>
-      <c r="B46" s="19" t="s">
-        <v>208</v>
-      </c>
-      <c r="E46" s="13" t="s">
-        <v>125</v>
-      </c>
-      <c r="F46" s="18" t="s">
-        <v>99</v>
-      </c>
-      <c r="G46" s="18" t="s">
+        <v>179</v>
+      </c>
+      <c r="B46" s="17" t="s">
+        <v>245</v>
+      </c>
+      <c r="D46" t="s">
+        <v>12</v>
+      </c>
+      <c r="F46" s="17" t="s">
+        <v>182</v>
+      </c>
+      <c r="G46" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="H46" s="17" t="s">
+        <v>191</v>
+      </c>
+      <c r="I46" s="17"/>
+      <c r="J46" s="17" t="str">
+        <f>CONCATENATE(A46, "=", F46, ",")</f>
+        <v>suceeding_interval=b12,</v>
+      </c>
+      <c r="K46" s="17" t="str">
+        <f>CONCATENATE("table(kr$", A46, ")")</f>
+        <v>table(kr$suceeding_interval)</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="17" t="s">
+        <v>224</v>
+      </c>
+      <c r="B47" s="17" t="s">
+        <v>225</v>
+      </c>
+      <c r="E47" s="17" t="s">
+        <v>193</v>
+      </c>
+      <c r="F47" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="G47" s="16" t="s">
         <v>139</v>
       </c>
-      <c r="H46" s="18" t="s">
-        <v>191</v>
-      </c>
-      <c r="I46" s="19"/>
-      <c r="J46" s="19" t="str">
-        <f t="shared" si="2"/>
-        <v>head_sex=hv219,</v>
-      </c>
-      <c r="K46" s="19" t="str">
-        <f t="shared" si="3"/>
-        <v>table(pr$head_sex)</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="15" t="s">
-        <v>85</v>
-      </c>
-      <c r="B47" s="19" t="s">
-        <v>216</v>
-      </c>
-      <c r="D47" s="15" t="s">
-        <v>217</v>
-      </c>
-      <c r="E47" s="15" t="s">
-        <v>126</v>
-      </c>
-      <c r="F47" s="18" t="s">
-        <v>127</v>
-      </c>
-      <c r="G47" s="18" t="s">
-        <v>139</v>
-      </c>
-      <c r="H47" s="18" t="s">
-        <v>191</v>
-      </c>
-      <c r="I47" s="19"/>
-      <c r="J47" s="19" t="str">
-        <f t="shared" si="2"/>
-        <v>head_age=hv220,</v>
-      </c>
-      <c r="K47" s="19" t="str">
-        <f t="shared" si="3"/>
-        <v>table(pr$head_age)</v>
+      <c r="H47" s="16" t="s">
+        <v>191</v>
+      </c>
+      <c r="J47" s="17" t="str">
+        <f>CONCATENATE(A47, "=", E47, ",")</f>
+        <v>toilet=hv205,</v>
+      </c>
+      <c r="K47" s="17" t="str">
+        <f>CONCATENATE("table(pr$", A47, ")")</f>
+        <v>table(pr$toilet)</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>95</v>
-      </c>
-      <c r="E48" t="s">
-        <v>164</v>
-      </c>
-      <c r="F48" s="19" t="s">
-        <v>96</v>
-      </c>
-      <c r="G48" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="B48" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="E48" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="F48" t="s">
+        <v>120</v>
+      </c>
+      <c r="G48" s="17" t="s">
         <v>139</v>
       </c>
-      <c r="H48" s="18" t="s">
-        <v>191</v>
-      </c>
-      <c r="I48" s="19"/>
-      <c r="J48" s="19" t="str">
-        <f t="shared" si="2"/>
-        <v>sampweight=hv005,</v>
-      </c>
-      <c r="K48" s="19" t="str">
-        <f t="shared" si="3"/>
-        <v>table(pr$sampweight)</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="19" t="s">
-        <v>232</v>
-      </c>
-      <c r="B49" s="19" t="s">
-        <v>233</v>
-      </c>
-      <c r="E49" s="19" t="s">
-        <v>193</v>
-      </c>
-      <c r="F49" s="19" t="s">
-        <v>106</v>
-      </c>
-      <c r="G49" s="18" t="s">
+      <c r="H48" s="17" t="s">
+        <v>191</v>
+      </c>
+      <c r="I48" s="17"/>
+      <c r="J48" t="str">
+        <f>CONCATENATE(A48, "=", E48, ",")</f>
+        <v>urban_rural=hv025,</v>
+      </c>
+      <c r="K48" t="str">
+        <f>CONCATENATE("table(pr$", A48, ")")</f>
+        <v>table(pr$urban_rural)</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>102</v>
+      </c>
+      <c r="B49" s="17" t="s">
+        <v>209</v>
+      </c>
+      <c r="C49" t="s">
+        <v>217</v>
+      </c>
+      <c r="D49" t="s">
+        <v>103</v>
+      </c>
+      <c r="E49" s="17" t="s">
+        <v>132</v>
+      </c>
+      <c r="F49" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="G49" s="17" t="s">
         <v>139</v>
       </c>
-      <c r="H49" s="18" t="s">
-        <v>191</v>
-      </c>
-      <c r="J49" s="19" t="str">
-        <f t="shared" si="2"/>
-        <v>toilet=hv205,</v>
-      </c>
-      <c r="K49" s="19" t="str">
-        <f t="shared" si="3"/>
-        <v>table(pr$toilet)</v>
+      <c r="H49" s="17" t="s">
+        <v>191</v>
+      </c>
+      <c r="I49" s="17"/>
+      <c r="J49" t="str">
+        <f>CONCATENATE(A49, "=", E49, ",")</f>
+        <v>watersource_dist=hv204,</v>
+      </c>
+      <c r="K49" t="str">
+        <f>CONCATENATE("table(pr$", A49, ")")</f>
+        <v>table(pr$watersource_dist)</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>188</v>
+        <v>19</v>
+      </c>
+      <c r="B50" s="17" t="s">
+        <v>246</v>
       </c>
       <c r="D50" t="s">
-        <v>217</v>
-      </c>
-      <c r="E50" s="19" t="s">
-        <v>230</v>
-      </c>
-      <c r="G50" s="19" t="s">
-        <v>177</v>
-      </c>
-      <c r="H50" s="19" t="s">
-        <v>191</v>
-      </c>
-      <c r="I50" s="19"/>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>189</v>
-      </c>
-      <c r="D51" t="s">
-        <v>217</v>
-      </c>
-      <c r="E51" s="19" t="s">
-        <v>230</v>
-      </c>
-      <c r="F51" s="19"/>
-      <c r="G51" s="19" t="s">
-        <v>177</v>
-      </c>
-      <c r="H51" s="19" t="s">
-        <v>191</v>
-      </c>
-      <c r="I51" s="19"/>
+        <v>203</v>
+      </c>
+      <c r="E50" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="F50" t="s">
+        <v>26</v>
+      </c>
+      <c r="G50" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="H50" s="17" t="s">
+        <v>191</v>
+      </c>
+      <c r="I50" s="17"/>
+      <c r="J50" t="str">
+        <f>CONCATENATE(A50, "=", E50, ",")</f>
+        <v>waz_dhs=hc8,</v>
+      </c>
+      <c r="K50" t="str">
+        <f>CONCATENATE("table(pr$", A50, ")")</f>
+        <v>table(pr$waz_dhs)</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B51" s="17" t="s">
+        <v>246</v>
+      </c>
+      <c r="D51" s="11" t="s">
+        <v>203</v>
+      </c>
+      <c r="E51" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="F51" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="G51" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="H51" s="17" t="s">
+        <v>191</v>
+      </c>
+      <c r="I51" s="17"/>
+      <c r="J51" s="11" t="str">
+        <f>CONCATENATE(A51, "=", E51, ",")</f>
+        <v>waz_who=hc71,</v>
+      </c>
+      <c r="K51" s="11" t="str">
+        <f>CONCATENATE("table(pr$", A51, ")")</f>
+        <v>table(pr$waz_who)</v>
+      </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>197</v>
-      </c>
-      <c r="E52" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="B52" s="17" t="s">
+        <v>247</v>
+      </c>
+      <c r="E52" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="F52" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="G52" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="H52" s="17" t="s">
+        <v>191</v>
+      </c>
+      <c r="I52" s="17"/>
+      <c r="J52" t="str">
+        <f>CONCATENATE(A52, "=", E52, ",")</f>
+        <v>wealth_factor=hv271,</v>
+      </c>
+      <c r="K52" t="str">
+        <f>CONCATENATE("table(pr$", A52, ")")</f>
+        <v>table(pr$wealth_factor)</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>49</v>
+      </c>
+      <c r="B53" s="17" t="s">
+        <v>208</v>
+      </c>
+      <c r="E53" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="F53" t="s">
+        <v>51</v>
+      </c>
+      <c r="G53" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="H53" s="17" t="s">
+        <v>191</v>
+      </c>
+      <c r="I53" s="13"/>
+      <c r="J53" t="str">
+        <f>CONCATENATE(A53, "=", E53, ",")</f>
+        <v>wealth_index=hv270,</v>
+      </c>
+      <c r="K53" t="str">
+        <f>CONCATENATE("table(pr$", A53, ")")</f>
+        <v>table(pr$wealth_index)</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B54" s="17" t="s">
+        <v>201</v>
+      </c>
+      <c r="D54" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="E54" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="F54" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="G54" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="H54" s="17" t="s">
+        <v>191</v>
+      </c>
+      <c r="J54" s="17" t="str">
+        <f>CONCATENATE(A54, "=", E54, ",")</f>
+        <v>weight=hc2,</v>
+      </c>
+      <c r="K54" s="17" t="str">
+        <f>CONCATENATE("table(pr$", A54, ")")</f>
+        <v>table(pr$weight)</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B55" s="17" t="s">
+        <v>246</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F55" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G55" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="H55" s="17" t="s">
+        <v>191</v>
+      </c>
+      <c r="I55" s="13"/>
+      <c r="J55" s="2" t="str">
+        <f>CONCATENATE(A55, "=", E55, ",")</f>
+        <v>whz_dhs=hc11,</v>
+      </c>
+      <c r="K55" s="2" t="str">
+        <f>CONCATENATE("table(pr$", A55, ")")</f>
+        <v>table(pr$whz_dhs)</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B56" s="17" t="s">
+        <v>246</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F56" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G56" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="H56" s="17" t="s">
+        <v>191</v>
+      </c>
+      <c r="I56" s="13"/>
+      <c r="J56" s="2" t="str">
+        <f>CONCATENATE(A56, "=", E56, ",")</f>
+        <v>whz_who=hc72,</v>
+      </c>
+      <c r="K56" s="2" t="str">
+        <f>CONCATENATE("table(pr$", A56, ")")</f>
+        <v>table(pr$whz_who)</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="B57" s="17" t="s">
+        <v>248</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="E57" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="G52" s="16" t="s">
+      <c r="G57" s="17" t="s">
         <v>177</v>
       </c>
-      <c r="H52" s="19" t="s">
-        <v>191</v>
-      </c>
-      <c r="I52" s="19"/>
-    </row>
-    <row r="53" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="B53" s="19"/>
-      <c r="E53" s="13" t="s">
-        <v>160</v>
-      </c>
-      <c r="G53" s="19" t="s">
-        <v>177</v>
-      </c>
-      <c r="H53" s="19" t="s">
-        <v>191</v>
-      </c>
-      <c r="I53" s="19"/>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>91</v>
-      </c>
-      <c r="E54" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="F54" s="5"/>
-      <c r="H54" s="19" t="s">
-        <v>192</v>
-      </c>
-      <c r="I54" s="19"/>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>234</v>
-      </c>
-      <c r="C55" t="s">
-        <v>236</v>
-      </c>
-      <c r="E55" s="19" t="s">
-        <v>160</v>
-      </c>
-      <c r="G55" s="19" t="s">
-        <v>177</v>
-      </c>
-      <c r="H55" s="19" t="s">
-        <v>191</v>
-      </c>
-      <c r="I55" s="15"/>
-    </row>
-    <row r="56" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="19" t="s">
-        <v>235</v>
-      </c>
-      <c r="C56" s="19" t="s">
-        <v>237</v>
-      </c>
-      <c r="E56" s="19" t="s">
-        <v>160</v>
-      </c>
-      <c r="G56" s="19" t="s">
-        <v>177</v>
-      </c>
-      <c r="H56" s="19" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="57" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="B57" s="19"/>
-      <c r="E57" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="F57" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="G57" s="19" t="s">
-        <v>175</v>
-      </c>
-      <c r="H57" s="18" t="s">
-        <v>192</v>
-      </c>
-      <c r="I57" s="15"/>
-    </row>
-    <row r="58" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B58" s="19"/>
-      <c r="E58" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="F58" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G58" s="19" t="s">
-        <v>175</v>
-      </c>
-      <c r="H58" s="18" t="s">
-        <v>192</v>
-      </c>
-      <c r="I58" s="15"/>
-    </row>
-    <row r="59" spans="1:11" s="3" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B59" s="19"/>
-      <c r="E59" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="F59" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="G59" s="19" t="s">
-        <v>139</v>
-      </c>
-      <c r="H59" s="18" t="s">
-        <v>192</v>
-      </c>
-      <c r="I59" s="15"/>
-    </row>
-    <row r="60" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="19"/>
-      <c r="G60" s="19"/>
-      <c r="H60" s="19"/>
-    </row>
-    <row r="61" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B61" s="19"/>
-      <c r="G61" s="19"/>
-      <c r="H61" s="19"/>
-    </row>
-    <row r="62" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B62" s="19"/>
-      <c r="G62" s="19"/>
-      <c r="H62" s="19"/>
-    </row>
-    <row r="63" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B63" s="19"/>
-      <c r="G63" s="19"/>
-      <c r="H63" s="19"/>
+      <c r="H57" s="17" t="s">
+        <v>191</v>
+      </c>
+      <c r="I57" s="13"/>
+    </row>
+    <row r="58" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B58" s="17"/>
+      <c r="G58" s="17"/>
+      <c r="H58" s="17"/>
+    </row>
+    <row r="59" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B59" s="17"/>
+      <c r="G59" s="17"/>
+      <c r="H59" s="17"/>
+    </row>
+    <row r="60" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="18"/>
+      <c r="B60" s="17"/>
+      <c r="G60" s="17"/>
+      <c r="H60" s="17"/>
+    </row>
+    <row r="61" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="18"/>
+      <c r="B61" s="17"/>
+      <c r="G61" s="17"/>
+      <c r="H61" s="17"/>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A62" s="19"/>
     </row>
   </sheetData>
-  <sortState ref="A1:K64">
-    <sortCondition ref="G1"/>
+  <sortState ref="A2:K59">
+    <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3226,378 +3282,378 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="17" t="s">
         <v>139</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="17" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="17" t="s">
         <v>129</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="17" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="17" t="s">
         <v>142</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="17" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="17" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="17" t="s">
         <v>143</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="17" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="17" t="s">
         <v>144</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="17" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="17" t="s">
         <v>131</v>
       </c>
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="17" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="17" t="s">
         <v>134</v>
       </c>
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="17" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="19" t="s">
+      <c r="A9" s="17" t="s">
         <v>130</v>
       </c>
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="17" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="19" t="s">
+      <c r="A10" s="17" t="s">
         <v>146</v>
       </c>
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="17" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="19" t="s">
+      <c r="A11" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="19" t="s">
+      <c r="B11" s="17" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="19" t="s">
+      <c r="A12" s="17" t="s">
         <v>147</v>
       </c>
-      <c r="B12" s="19" t="s">
+      <c r="B12" s="17" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="19" t="s">
+      <c r="A13" s="17" t="s">
         <v>148</v>
       </c>
-      <c r="B13" s="19" t="s">
+      <c r="B13" s="17" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="19" t="s">
+      <c r="A14" s="17" t="s">
         <v>149</v>
       </c>
-      <c r="B14" s="19" t="s">
+      <c r="B14" s="17" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="19" t="s">
+      <c r="A15" s="17" t="s">
         <v>150</v>
       </c>
-      <c r="B15" s="19" t="s">
+      <c r="B15" s="17" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="19" t="s">
+      <c r="A16" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="B16" s="19" t="s">
+      <c r="B16" s="17" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="19" t="s">
+      <c r="A17" s="17" t="s">
         <v>151</v>
       </c>
-      <c r="B17" s="19" t="s">
+      <c r="B17" s="17" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="19" t="s">
+      <c r="A18" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="B18" s="19" t="s">
+      <c r="B18" s="17" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="19" t="s">
+      <c r="A19" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="B19" s="19" t="s">
+      <c r="B19" s="17" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="19" t="s">
+      <c r="A20" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="B20" s="19" t="s">
+      <c r="B20" s="17" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="19" t="s">
+      <c r="A21" s="17" t="s">
         <v>152</v>
       </c>
-      <c r="B21" s="19" t="s">
+      <c r="B21" s="17" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="19" t="s">
+      <c r="A22" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="B22" s="19" t="s">
+      <c r="B22" s="17" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="19" t="s">
+      <c r="A23" s="17" t="s">
         <v>153</v>
       </c>
-      <c r="B23" s="19" t="s">
+      <c r="B23" s="17" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="19" t="s">
+      <c r="A24" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="B24" s="19" t="s">
+      <c r="B24" s="17" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="19" t="s">
+      <c r="A25" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="B25" s="19" t="s">
+      <c r="B25" s="17" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="19" t="s">
+      <c r="A26" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="B26" s="19" t="s">
+      <c r="B26" s="17" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="19" t="s">
+      <c r="A27" s="17" t="s">
         <v>154</v>
       </c>
-      <c r="B27" s="19" t="s">
+      <c r="B27" s="17" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="19" t="s">
+      <c r="A28" s="17" t="s">
         <v>155</v>
       </c>
-      <c r="B28" s="19" t="s">
+      <c r="B28" s="17" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="19" t="s">
+      <c r="A29" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="B29" s="19" t="s">
+      <c r="B29" s="17" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="19" t="s">
+      <c r="A30" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="B30" s="19" t="s">
+      <c r="B30" s="17" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="19" t="s">
+      <c r="A31" s="17" t="s">
         <v>135</v>
       </c>
-      <c r="B31" s="19" t="s">
+      <c r="B31" s="17" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="19" t="s">
+      <c r="A32" s="17" t="s">
         <v>156</v>
       </c>
-      <c r="B32" s="19" t="s">
+      <c r="B32" s="17" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="19" t="s">
+      <c r="A33" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="B33" s="19" t="s">
+      <c r="B33" s="17" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="19" t="s">
+      <c r="A34" s="17" t="s">
         <v>157</v>
       </c>
-      <c r="B34" s="19" t="s">
+      <c r="B34" s="17" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="19" t="s">
+      <c r="A35" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="B35" s="19" t="s">
+      <c r="B35" s="17" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="19" t="s">
+      <c r="A36" s="17" t="s">
         <v>159</v>
       </c>
-      <c r="B36" s="19" t="s">
+      <c r="B36" s="17" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="19" t="s">
+      <c r="A37" s="17" t="s">
         <v>160</v>
       </c>
-      <c r="B37" s="19" t="s">
+      <c r="B37" s="17" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="19" t="s">
+      <c r="A38" s="17" t="s">
         <v>138</v>
       </c>
-      <c r="B38" s="19" t="s">
+      <c r="B38" s="17" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="19" t="s">
+      <c r="A39" s="17" t="s">
         <v>136</v>
       </c>
-      <c r="B39" s="19" t="s">
+      <c r="B39" s="17" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="19" t="s">
+      <c r="A40" s="17" t="s">
         <v>137</v>
       </c>
-      <c r="B40" s="19" t="s">
+      <c r="B40" s="17" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="19" t="s">
+      <c r="A41" s="17" t="s">
         <v>125</v>
       </c>
-      <c r="B41" s="19" t="s">
+      <c r="B41" s="17" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="19" t="s">
+      <c r="A42" s="17" t="s">
         <v>126</v>
       </c>
-      <c r="B42" s="19" t="s">
+      <c r="B42" s="17" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="19" t="s">
+      <c r="A43" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="B43" s="19" t="s">
+      <c r="B43" s="17" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="19" t="s">
+      <c r="A44" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="B44" s="19"/>
+      <c r="B44" s="17"/>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="19" t="s">
+      <c r="A45" s="17" t="s">
         <v>150</v>
       </c>
-      <c r="B45" s="19"/>
+      <c r="B45" s="17"/>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="19" t="s">
+      <c r="A46" s="17" t="s">
         <v>161</v>
       </c>
-      <c r="B46" s="19"/>
+      <c r="B46" s="17"/>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="19" t="s">
+      <c r="A47" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="B47" s="19"/>
+      <c r="B47" s="17"/>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="19" t="s">
+      <c r="A48" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="B48" s="19"/>
+      <c r="B48" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3614,15 +3670,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.28515625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="21.28515625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>77</v>
       </c>
       <c r="C1" t="str">
@@ -3631,531 +3687,531 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C2" s="3" t="str">
+      <c r="C2" s="2" t="str">
         <f t="shared" ref="C2:C36" si="0">CONCATENATE(A2, "=", B2, ",")</f>
         <v>sex=b4,</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="C3" s="3" t="str">
+      <c r="C3" s="2" t="str">
         <f t="shared" si="0"/>
         <v>birth_order=bord,</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="14" t="s">
         <v>121</v>
       </c>
-      <c r="C4" s="3" t="str">
+      <c r="C4" s="2" t="str">
         <f t="shared" si="0"/>
         <v>birth_order=midx,</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="3" t="str">
+      <c r="C5" s="2" t="str">
         <f t="shared" si="0"/>
         <v>caseid=caseid,</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="16" t="s">
         <v>100</v>
       </c>
-      <c r="C6" s="3" t="str">
+      <c r="C6" s="2" t="str">
         <f t="shared" si="0"/>
         <v>diarrhea=h11,</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="C7" s="3" t="str">
+      <c r="C7" s="2" t="str">
         <f t="shared" si="0"/>
         <v>fever=h22,</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="C8" s="3" t="str">
+      <c r="C8" s="2" t="str">
         <f t="shared" si="0"/>
         <v>parasite_drugs=h43,</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="C9" s="3" t="str">
+      <c r="C9" s="2" t="str">
         <f t="shared" si="0"/>
         <v>age=hw1,</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="3" t="str">
+      <c r="C10" s="2" t="str">
         <f t="shared" si="0"/>
         <v>whz_dhs=hw11,</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="C11" s="3" t="str">
+      <c r="C11" s="2" t="str">
         <f t="shared" si="0"/>
         <v>weight=hw2,</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="C12" s="3" t="str">
+      <c r="C12" s="2" t="str">
         <f t="shared" si="0"/>
         <v>height=hw3,</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="3" t="str">
+      <c r="C13" s="2" t="str">
         <f t="shared" si="0"/>
         <v>haz_dhs=hw5,</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C14" s="3" t="str">
+      <c r="C14" s="2" t="str">
         <f t="shared" si="0"/>
         <v>haz_who=hw70,</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C15" s="3" t="str">
+      <c r="C15" s="2" t="str">
         <f t="shared" si="0"/>
         <v>waz_who=hw71,</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C16" s="3" t="str">
+      <c r="C16" s="2" t="str">
         <f t="shared" si="0"/>
         <v>whz_who=hw72,</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C17" s="3" t="str">
+      <c r="C17" s="2" t="str">
         <f t="shared" si="0"/>
         <v>waz_dhs=hw8,</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="C18" s="3" t="str">
+      <c r="C18" s="2" t="str">
         <f t="shared" si="0"/>
         <v>birth_weight=m19,</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C19" s="3" t="str">
+      <c r="C19" s="2" t="str">
         <f t="shared" si="0"/>
         <v>breast_duration=m4,</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C20" s="3" t="str">
+      <c r="C20" s="2" t="str">
         <f t="shared" si="0"/>
         <v>hhid=v002,</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
+      <c r="A21" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="C21" s="3" t="str">
+      <c r="C21" s="2" t="str">
         <f t="shared" si="0"/>
         <v>rlinenum=v003,</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
+      <c r="A22" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="C22" s="3" t="str">
+      <c r="C22" s="2" t="str">
         <f t="shared" si="0"/>
         <v>sampweight=v005,</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
+      <c r="A23" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B23" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C23" s="3" t="str">
+      <c r="C23" s="2" t="str">
         <f t="shared" si="0"/>
         <v>month=v006,</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
+      <c r="A24" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C24" s="3" t="str">
+      <c r="C24" s="2" t="str">
         <f t="shared" si="0"/>
         <v>year=v007,</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
+      <c r="A25" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="B25" s="17" t="s">
+      <c r="B25" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="C25" s="3" t="str">
+      <c r="C25" s="2" t="str">
         <f t="shared" si="0"/>
         <v>interview_cmc=v008,</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
+      <c r="A26" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="B26" s="17" t="s">
+      <c r="B26" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="C26" s="3" t="str">
+      <c r="C26" s="2" t="str">
         <f t="shared" si="0"/>
         <v>birthmonth=v009,</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
+      <c r="A27" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="B27" s="17" t="s">
+      <c r="B27" s="15" t="s">
         <v>116</v>
       </c>
-      <c r="C27" s="3" t="str">
+      <c r="C27" s="2" t="str">
         <f t="shared" si="0"/>
         <v>birthyear=v010,</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
+      <c r="A28" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B28" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="C28" s="3" t="str">
+      <c r="C28" s="2" t="str">
         <f t="shared" si="0"/>
         <v>birthday_cmc=V011,</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
+      <c r="A29" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B29" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="C29" s="3" t="str">
+      <c r="C29" s="2" t="str">
         <f t="shared" si="0"/>
         <v>urban_rural=v025,</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
+      <c r="A30" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="B30" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C30" s="3" t="str">
+      <c r="C30" s="2" t="str">
         <f t="shared" si="0"/>
         <v>watersource=v113,</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
+      <c r="A31" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="B31" s="18" t="s">
+      <c r="B31" s="16" t="s">
         <v>104</v>
       </c>
-      <c r="C31" s="3" t="str">
+      <c r="C31" s="2" t="str">
         <f t="shared" si="0"/>
         <v>watersource_dist=v115,</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
+      <c r="A32" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B32" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="C32" s="3" t="str">
+      <c r="C32" s="2" t="str">
         <f t="shared" si="0"/>
         <v>sanitation_facility=v116,</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
+      <c r="A33" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B33" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C33" s="3" t="str">
+      <c r="C33" s="2" t="str">
         <f t="shared" si="0"/>
         <v>hhsize=v136,</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
+      <c r="A34" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B34" s="18" t="s">
+      <c r="B34" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="C34" s="3" t="str">
+      <c r="C34" s="2" t="str">
         <f t="shared" si="0"/>
         <v>head_sex=v151,</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
+      <c r="A35" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="B35" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C35" s="3" t="str">
+      <c r="C35" s="2" t="str">
         <f t="shared" si="0"/>
         <v>wealth_index=v190,</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
+      <c r="A36" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="B36" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C36" s="3" t="str">
+      <c r="C36" s="2" t="str">
         <f t="shared" si="0"/>
         <v>wealth_factor=v191,</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="s">
+      <c r="A37" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
+      <c r="A38" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="3" t="s">
+      <c r="A39" s="2" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
+      <c r="A40" s="2" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="3" t="s">
+      <c r="A41" s="2" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="3" t="s">
+      <c r="A42" s="2" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="3" t="s">
+      <c r="A43" s="2" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="3" t="s">
+      <c r="A44" s="2" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="3" t="s">
+      <c r="A45" s="2" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="3" t="s">
+      <c r="A46" s="2" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="3" t="s">
+      <c r="A47" s="2" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="3" t="s">
+      <c r="A48" s="2" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="3" t="s">
+      <c r="A49" s="2" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="3" t="s">
+      <c r="A53" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B53" s="3" t="s">
+      <c r="B53" s="2" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="3" t="s">
+      <c r="A54" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B54" s="3" t="s">
+      <c r="B54" s="2" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="3" t="s">
+      <c r="A55" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B55" s="3" t="s">
+      <c r="B55" s="2" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="3" t="s">
+      <c r="A56" s="2" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="3" t="s">
+      <c r="A57" s="2" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="3" t="s">
+      <c r="A58" s="2" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="3" t="s">
+      <c r="A59" s="2" t="s">
         <v>111</v>
       </c>
     </row>

</xml_diff>